<commit_message>
more implementation of prior period validations
</commit_message>
<xml_diff>
--- a/tests/server/fixtures/file-success/EOHHS-075-12312020-simple-v1.xlsx
+++ b/tests/server/fixtures/file-success/EOHHS-075-12312020-simple-v1.xlsx
@@ -1318,7 +1318,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1370,7 +1370,9 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="8" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="4" fillId="8" fontId="4" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="4" fillId="8" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="3" fillId="8" fontId="4" numFmtId="14" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -1394,6 +1396,7 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="4" fillId="8" fontId="4" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="1" fillId="8" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="7" fillId="8" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -7996,10 +7999,10 @@
       <c r="C3" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D3" s="48">
+      <c r="D3" s="49">
         <v>2163121.97</v>
       </c>
-      <c r="E3" s="48">
+      <c r="E3" s="49">
         <v>840542.45</v>
       </c>
     </row>
@@ -8013,10 +8016,10 @@
       <c r="C4" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D4" s="48">
+      <c r="D4" s="49">
         <v>5957909.0</v>
       </c>
-      <c r="E4" s="48">
+      <c r="E4" s="49">
         <v>5957909.0</v>
       </c>
     </row>
@@ -9071,10 +9074,10 @@
       <c r="B2" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C2" s="43">
+      <c r="C2" s="44">
         <v>1567999.5</v>
       </c>
-      <c r="D2" s="43">
+      <c r="D2" s="44">
         <v>1567999.5</v>
       </c>
     </row>
@@ -10101,119 +10104,119 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>222</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="50" t="s">
         <v>223</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="50" t="s">
         <v>224</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="50" t="s">
         <v>224</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="50" t="s">
         <v>214</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="50" t="s">
         <v>224</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="50" t="s">
         <v>225</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="I1" s="50" t="s">
         <v>215</v>
       </c>
-      <c r="J1" s="49" t="s">
+      <c r="J1" s="50" t="s">
         <v>215</v>
       </c>
-      <c r="K1" s="49" t="s">
+      <c r="K1" s="50" t="s">
         <v>217</v>
       </c>
-      <c r="L1" s="49" t="s">
+      <c r="L1" s="50" t="s">
         <v>226</v>
       </c>
-      <c r="M1" s="49" t="s">
+      <c r="M1" s="50" t="s">
         <v>226</v>
       </c>
-      <c r="N1" s="49" t="s">
+      <c r="N1" s="50" t="s">
         <v>227</v>
       </c>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
-      <c r="S1" s="49"/>
-      <c r="T1" s="49"/>
-      <c r="U1" s="49"/>
-      <c r="V1" s="49"/>
-      <c r="W1" s="49"/>
-      <c r="X1" s="49"/>
-      <c r="Y1" s="49"/>
-      <c r="Z1" s="49"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="50"/>
     </row>
     <row r="2" ht="15.0" customHeight="1">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="50" t="s">
         <v>228</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="51" t="s">
         <v>229</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="G2" s="50" t="s">
+      <c r="G2" s="51" t="s">
         <v>230</v>
       </c>
-      <c r="H2" s="50" t="s">
+      <c r="H2" s="51" t="s">
         <v>231</v>
       </c>
-      <c r="I2" s="50" t="s">
+      <c r="I2" s="51" t="s">
         <v>170</v>
       </c>
-      <c r="J2" s="50" t="s">
+      <c r="J2" s="51" t="s">
         <v>232</v>
       </c>
-      <c r="K2" s="50" t="s">
+      <c r="K2" s="51" t="s">
         <v>194</v>
       </c>
-      <c r="L2" s="50" t="s">
+      <c r="L2" s="51" t="s">
         <v>211</v>
       </c>
-      <c r="M2" s="50" t="s">
+      <c r="M2" s="51" t="s">
         <v>212</v>
       </c>
-      <c r="N2" s="50" t="s">
+      <c r="N2" s="51" t="s">
         <v>212</v>
       </c>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="49"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
-      <c r="V2" s="49"/>
-      <c r="W2" s="49"/>
-      <c r="X2" s="49"/>
-      <c r="Y2" s="49"/>
-      <c r="Z2" s="49"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="50"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="50"/>
+      <c r="X2" s="50"/>
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="50"/>
     </row>
     <row r="3" ht="15.0" customHeight="1">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="50" t="s">
         <v>233</v>
       </c>
       <c r="B3" s="18" t="s">
@@ -10313,7 +10316,7 @@
       <c r="F5" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="G5" s="51" t="s">
+      <c r="G5" s="52" t="s">
         <v>251</v>
       </c>
       <c r="L5" s="18" t="s">
@@ -10355,7 +10358,7 @@
       <c r="D8" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="E8" s="52" t="s">
+      <c r="E8" s="53" t="s">
         <v>259</v>
       </c>
     </row>
@@ -11644,102 +11647,102 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="2" ht="15.0" customHeight="1">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="54" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="1">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="54" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="4" ht="15.0" customHeight="1">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="54" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" ht="15.0" customHeight="1">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="54" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="1">
-      <c r="A7" s="49"/>
-      <c r="B7" s="49" t="s">
+      <c r="A7" s="50"/>
+      <c r="B7" s="50" t="s">
         <v>325</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49" t="s">
+      <c r="C7" s="50"/>
+      <c r="D7" s="50" t="s">
         <v>326</v>
       </c>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49" t="s">
+      <c r="E7" s="50"/>
+      <c r="F7" s="50" t="s">
         <v>327</v>
       </c>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="49"/>
-      <c r="O7" s="49"/>
-      <c r="P7" s="49"/>
-      <c r="Q7" s="49"/>
-      <c r="R7" s="49"/>
-      <c r="S7" s="49"/>
-      <c r="T7" s="49"/>
-      <c r="U7" s="49"/>
-      <c r="V7" s="49"/>
-      <c r="W7" s="49"/>
-      <c r="X7" s="49"/>
-      <c r="Y7" s="49"/>
-      <c r="Z7" s="49"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="50"/>
+      <c r="R7" s="50"/>
+      <c r="S7" s="50"/>
+      <c r="T7" s="50"/>
+      <c r="U7" s="50"/>
+      <c r="V7" s="50"/>
+      <c r="W7" s="50"/>
+      <c r="X7" s="50"/>
+      <c r="Y7" s="50"/>
+      <c r="Z7" s="50"/>
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="18" t="s">
         <v>328</v>
       </c>
-      <c r="B8" s="54"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="55"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="56"/>
     </row>
     <row r="9" ht="15.0" customHeight="1">
       <c r="A9" s="18" t="s">
         <v>329</v>
       </c>
-      <c r="B9" s="54"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="55"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="56"/>
     </row>
     <row r="10" ht="15.0" customHeight="1">
       <c r="A10" s="18" t="s">
         <v>330</v>
       </c>
-      <c r="B10" s="55"/>
-      <c r="C10" s="54">
+      <c r="B10" s="56"/>
+      <c r="C10" s="55">
         <f>B8+B9</f>
         <v>0</v>
       </c>
-      <c r="D10" s="55"/>
-      <c r="E10" s="54">
+      <c r="D10" s="56"/>
+      <c r="E10" s="55">
         <f>D8+D9</f>
         <v>0</v>
       </c>
-      <c r="F10" s="55"/>
-      <c r="G10" s="54">
+      <c r="F10" s="56"/>
+      <c r="G10" s="55">
         <f>F8+F9</f>
         <v>0</v>
       </c>
@@ -11748,40 +11751,40 @@
       <c r="A11" s="18" t="s">
         <v>331</v>
       </c>
-      <c r="B11" s="54"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="55"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="56"/>
     </row>
     <row r="12" ht="15.0" customHeight="1">
       <c r="A12" s="18" t="s">
         <v>332</v>
       </c>
-      <c r="B12" s="54"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="55"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="56"/>
     </row>
     <row r="13" ht="15.0" customHeight="1">
       <c r="A13" s="18" t="s">
         <v>333</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="54">
+      <c r="B13" s="56"/>
+      <c r="C13" s="55">
         <f>B11+B12</f>
         <v>0</v>
       </c>
-      <c r="D13" s="55"/>
-      <c r="E13" s="54">
+      <c r="D13" s="56"/>
+      <c r="E13" s="55">
         <f>D11+D12</f>
         <v>0</v>
       </c>
-      <c r="F13" s="55"/>
-      <c r="G13" s="54">
+      <c r="F13" s="56"/>
+      <c r="G13" s="55">
         <f>F11+F12</f>
         <v>0</v>
       </c>
@@ -11790,40 +11793,40 @@
       <c r="A14" s="18" t="s">
         <v>334</v>
       </c>
-      <c r="B14" s="54"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="55"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="56"/>
     </row>
     <row r="15" ht="15.0" customHeight="1">
       <c r="A15" s="18" t="s">
         <v>335</v>
       </c>
-      <c r="B15" s="54"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="55"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="56"/>
     </row>
     <row r="16" ht="15.0" customHeight="1">
       <c r="A16" s="18" t="s">
         <v>336</v>
       </c>
-      <c r="B16" s="55"/>
-      <c r="C16" s="54">
+      <c r="B16" s="56"/>
+      <c r="C16" s="55">
         <f>B14+B15</f>
         <v>0</v>
       </c>
-      <c r="D16" s="55"/>
-      <c r="E16" s="54">
+      <c r="D16" s="56"/>
+      <c r="E16" s="55">
         <f>D14+D15</f>
         <v>0</v>
       </c>
-      <c r="F16" s="55"/>
-      <c r="G16" s="54">
+      <c r="F16" s="56"/>
+      <c r="G16" s="55">
         <f>F14+F15</f>
         <v>0</v>
       </c>
@@ -11832,40 +11835,40 @@
       <c r="A17" s="18" t="s">
         <v>337</v>
       </c>
-      <c r="B17" s="54"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="55"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="56"/>
     </row>
     <row r="18" ht="15.0" customHeight="1">
       <c r="A18" s="18" t="s">
         <v>338</v>
       </c>
-      <c r="B18" s="54"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="55"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="56"/>
     </row>
     <row r="19" ht="15.0" customHeight="1">
       <c r="A19" s="18" t="s">
         <v>339</v>
       </c>
-      <c r="B19" s="55"/>
-      <c r="C19" s="54">
+      <c r="B19" s="56"/>
+      <c r="C19" s="55">
         <f>B17+B18</f>
         <v>0</v>
       </c>
-      <c r="D19" s="55"/>
-      <c r="E19" s="54">
+      <c r="D19" s="56"/>
+      <c r="E19" s="55">
         <f>D17+D18</f>
         <v>0</v>
       </c>
-      <c r="F19" s="55"/>
-      <c r="G19" s="54">
+      <c r="F19" s="56"/>
+      <c r="G19" s="55">
         <f>F17+F18</f>
         <v>0</v>
       </c>
@@ -11874,40 +11877,40 @@
       <c r="A20" s="18" t="s">
         <v>340</v>
       </c>
-      <c r="B20" s="54"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="55"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="56"/>
     </row>
     <row r="21" ht="15.0" customHeight="1">
       <c r="A21" s="18" t="s">
         <v>341</v>
       </c>
-      <c r="B21" s="54"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="55"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="56"/>
     </row>
     <row r="22" ht="15.0" customHeight="1">
       <c r="A22" s="18" t="s">
         <v>342</v>
       </c>
-      <c r="B22" s="55"/>
-      <c r="C22" s="54">
+      <c r="B22" s="56"/>
+      <c r="C22" s="55">
         <f>B20+B21</f>
         <v>0</v>
       </c>
-      <c r="D22" s="55"/>
-      <c r="E22" s="54">
+      <c r="D22" s="56"/>
+      <c r="E22" s="55">
         <f>D20+D21</f>
         <v>0</v>
       </c>
-      <c r="F22" s="55"/>
-      <c r="G22" s="54">
+      <c r="F22" s="56"/>
+      <c r="G22" s="55">
         <f>F20+F21</f>
         <v>0</v>
       </c>
@@ -11916,51 +11919,51 @@
       <c r="A23" s="18" t="s">
         <v>343</v>
       </c>
-      <c r="B23" s="55"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="54"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="55"/>
     </row>
     <row r="24" ht="15.0" customHeight="1">
-      <c r="A24" s="49" t="s">
+      <c r="A24" s="50" t="s">
         <v>344</v>
       </c>
-      <c r="B24" s="56"/>
-      <c r="C24" s="56">
+      <c r="B24" s="57"/>
+      <c r="C24" s="57">
         <f>C10+C13+C16+C19+C22</f>
         <v>0</v>
       </c>
-      <c r="D24" s="56"/>
-      <c r="E24" s="56">
+      <c r="D24" s="57"/>
+      <c r="E24" s="57">
         <f>E10+E13+E16+E19+E22</f>
         <v>0</v>
       </c>
-      <c r="F24" s="56"/>
-      <c r="G24" s="56">
+      <c r="F24" s="57"/>
+      <c r="G24" s="57">
         <f>G10+G13+G16+G19+G22</f>
         <v>0</v>
       </c>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="49"/>
-      <c r="O24" s="49"/>
-      <c r="P24" s="49"/>
-      <c r="Q24" s="49"/>
-      <c r="R24" s="49"/>
-      <c r="S24" s="49"/>
-      <c r="T24" s="49"/>
-      <c r="U24" s="49"/>
-      <c r="V24" s="49"/>
-      <c r="W24" s="49"/>
-      <c r="X24" s="49"/>
-      <c r="Y24" s="49"/>
-      <c r="Z24" s="49"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="50"/>
+      <c r="L24" s="50"/>
+      <c r="M24" s="50"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="50"/>
+      <c r="P24" s="50"/>
+      <c r="Q24" s="50"/>
+      <c r="R24" s="50"/>
+      <c r="S24" s="50"/>
+      <c r="T24" s="50"/>
+      <c r="U24" s="50"/>
+      <c r="V24" s="50"/>
+      <c r="W24" s="50"/>
+      <c r="X24" s="50"/>
+      <c r="Y24" s="50"/>
+      <c r="Z24" s="50"/>
     </row>
     <row r="25" ht="15.75" customHeight="1"/>
     <row r="26" ht="15.75" customHeight="1"/>
@@ -20314,7 +20317,7 @@
         <v>160</v>
       </c>
       <c r="E2" s="23">
-        <v>1376.0</v>
+        <v>51376.0</v>
       </c>
       <c r="F2" s="24">
         <v>43957.29016203704</v>
@@ -20466,7 +20469,7 @@
       <c r="D4" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="37">
         <v>27620.0</v>
       </c>
       <c r="F4" s="24">
@@ -20501,7 +20504,7 @@
       <c r="R4" s="13">
         <v>75.0</v>
       </c>
-      <c r="S4" s="23">
+      <c r="S4" s="37">
         <v>27620.0</v>
       </c>
       <c r="T4" s="24">
@@ -23172,7 +23175,7 @@
       <c r="D2" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="37">
         <v>2927600.0</v>
       </c>
       <c r="F2" s="24">
@@ -23201,13 +23204,13 @@
       <c r="O2" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="R2" s="37" t="s">
+      <c r="R2" s="38" t="s">
         <v>181</v>
       </c>
       <c r="T2" s="36">
         <v>75.0</v>
       </c>
-      <c r="U2" s="23">
+      <c r="U2" s="37">
         <v>2927600.0</v>
       </c>
       <c r="V2" s="24">
@@ -27897,7 +27900,7 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>69</v>
       </c>
       <c r="B2" s="22" t="s">
@@ -27936,7 +27939,7 @@
       <c r="M2" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="37" t="s">
+      <c r="O2" s="38" t="s">
         <v>196</v>
       </c>
       <c r="P2" s="22">
@@ -27953,7 +27956,7 @@
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>89</v>
       </c>
       <c r="B3" s="30" t="s">
@@ -27990,7 +27993,7 @@
       <c r="M3" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="O3" s="37" t="s">
+      <c r="O3" s="38" t="s">
         <v>196</v>
       </c>
       <c r="P3" s="30">
@@ -28007,7 +28010,7 @@
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="39" t="s">
         <v>63</v>
       </c>
       <c r="B4" s="22" t="s">
@@ -28046,7 +28049,7 @@
       <c r="M4" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="O4" s="37" t="s">
+      <c r="O4" s="38" t="s">
         <v>196</v>
       </c>
       <c r="P4" s="22">
@@ -28063,7 +28066,7 @@
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="39"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="30"/>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -28076,12 +28079,12 @@
       <c r="K5" s="30"/>
       <c r="L5" s="30"/>
       <c r="M5" s="30"/>
-      <c r="O5" s="37"/>
+      <c r="O5" s="38"/>
       <c r="P5" s="30"/>
       <c r="AC5" s="30"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="38"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
@@ -28094,12 +28097,12 @@
       <c r="K6" s="22"/>
       <c r="L6" s="22"/>
       <c r="M6" s="22"/>
-      <c r="O6" s="37"/>
+      <c r="O6" s="38"/>
       <c r="P6" s="22"/>
       <c r="AC6" s="22"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="39"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="30"/>
       <c r="C7" s="30"/>
       <c r="D7" s="30"/>
@@ -28112,12 +28115,12 @@
       <c r="K7" s="30"/>
       <c r="L7" s="30"/>
       <c r="M7" s="30"/>
-      <c r="O7" s="37"/>
+      <c r="O7" s="38"/>
       <c r="P7" s="30"/>
       <c r="AC7" s="30"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="38"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -28130,12 +28133,12 @@
       <c r="K8" s="22"/>
       <c r="L8" s="22"/>
       <c r="M8" s="22"/>
-      <c r="O8" s="37"/>
+      <c r="O8" s="38"/>
       <c r="P8" s="22"/>
       <c r="AC8" s="22"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="39"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="30"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
@@ -28148,12 +28151,12 @@
       <c r="K9" s="30"/>
       <c r="L9" s="30"/>
       <c r="M9" s="30"/>
-      <c r="O9" s="37"/>
+      <c r="O9" s="38"/>
       <c r="P9" s="30"/>
       <c r="AC9" s="30"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="38"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
@@ -28166,12 +28169,12 @@
       <c r="K10" s="22"/>
       <c r="L10" s="22"/>
       <c r="M10" s="22"/>
-      <c r="O10" s="37"/>
+      <c r="O10" s="38"/>
       <c r="P10" s="22"/>
       <c r="AC10" s="22"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="39"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="30"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
@@ -28184,12 +28187,12 @@
       <c r="K11" s="30"/>
       <c r="L11" s="30"/>
       <c r="M11" s="30"/>
-      <c r="O11" s="37"/>
+      <c r="O11" s="38"/>
       <c r="P11" s="30"/>
       <c r="AC11" s="30"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="38"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -28202,12 +28205,12 @@
       <c r="K12" s="22"/>
       <c r="L12" s="22"/>
       <c r="M12" s="22"/>
-      <c r="O12" s="37"/>
+      <c r="O12" s="38"/>
       <c r="P12" s="22"/>
       <c r="AC12" s="22"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="39"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="30"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -28220,12 +28223,12 @@
       <c r="K13" s="30"/>
       <c r="L13" s="30"/>
       <c r="M13" s="30"/>
-      <c r="O13" s="37"/>
+      <c r="O13" s="38"/>
       <c r="P13" s="30"/>
       <c r="AC13" s="30"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="38"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="22"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
@@ -28238,12 +28241,12 @@
       <c r="K14" s="22"/>
       <c r="L14" s="22"/>
       <c r="M14" s="22"/>
-      <c r="O14" s="37"/>
+      <c r="O14" s="38"/>
       <c r="P14" s="22"/>
       <c r="AC14" s="22"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="39"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="30"/>
       <c r="C15" s="30"/>
       <c r="D15" s="30"/>
@@ -28256,12 +28259,12 @@
       <c r="K15" s="30"/>
       <c r="L15" s="30"/>
       <c r="M15" s="30"/>
-      <c r="O15" s="37"/>
+      <c r="O15" s="38"/>
       <c r="P15" s="30"/>
       <c r="AC15" s="30"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="38"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
@@ -28274,12 +28277,12 @@
       <c r="K16" s="22"/>
       <c r="L16" s="22"/>
       <c r="M16" s="22"/>
-      <c r="O16" s="37"/>
+      <c r="O16" s="38"/>
       <c r="P16" s="22"/>
       <c r="AC16" s="22"/>
     </row>
     <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" s="39"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="30"/>
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
@@ -28292,12 +28295,12 @@
       <c r="K17" s="30"/>
       <c r="L17" s="30"/>
       <c r="M17" s="30"/>
-      <c r="O17" s="37"/>
+      <c r="O17" s="38"/>
       <c r="P17" s="30"/>
       <c r="AC17" s="30"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="38"/>
+      <c r="A18" s="39"/>
       <c r="B18" s="22"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
@@ -28310,12 +28313,12 @@
       <c r="K18" s="22"/>
       <c r="L18" s="22"/>
       <c r="M18" s="22"/>
-      <c r="O18" s="37"/>
+      <c r="O18" s="38"/>
       <c r="P18" s="22"/>
       <c r="AC18" s="22"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="39"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="30"/>
       <c r="C19" s="30"/>
       <c r="D19" s="30"/>
@@ -28328,12 +28331,12 @@
       <c r="K19" s="30"/>
       <c r="L19" s="30"/>
       <c r="M19" s="30"/>
-      <c r="O19" s="37"/>
+      <c r="O19" s="38"/>
       <c r="P19" s="30"/>
       <c r="AC19" s="30"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="38"/>
+      <c r="A20" s="39"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
@@ -28346,12 +28349,12 @@
       <c r="K20" s="22"/>
       <c r="L20" s="22"/>
       <c r="M20" s="22"/>
-      <c r="O20" s="37"/>
+      <c r="O20" s="38"/>
       <c r="P20" s="22"/>
       <c r="AC20" s="22"/>
     </row>
     <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="39"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="30"/>
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
@@ -28364,12 +28367,12 @@
       <c r="K21" s="30"/>
       <c r="L21" s="30"/>
       <c r="M21" s="30"/>
-      <c r="O21" s="37"/>
+      <c r="O21" s="38"/>
       <c r="P21" s="30"/>
       <c r="AC21" s="30"/>
     </row>
     <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" s="38"/>
+      <c r="A22" s="39"/>
       <c r="B22" s="22"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
@@ -28382,12 +28385,12 @@
       <c r="K22" s="22"/>
       <c r="L22" s="22"/>
       <c r="M22" s="22"/>
-      <c r="O22" s="37"/>
+      <c r="O22" s="38"/>
       <c r="P22" s="22"/>
       <c r="AC22" s="22"/>
     </row>
     <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="39"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="30"/>
       <c r="C23" s="30"/>
       <c r="D23" s="30"/>
@@ -28400,12 +28403,12 @@
       <c r="K23" s="30"/>
       <c r="L23" s="30"/>
       <c r="M23" s="30"/>
-      <c r="O23" s="37"/>
+      <c r="O23" s="38"/>
       <c r="P23" s="30"/>
       <c r="AC23" s="30"/>
     </row>
     <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" s="38"/>
+      <c r="A24" s="39"/>
       <c r="B24" s="22"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
@@ -28418,12 +28421,12 @@
       <c r="K24" s="22"/>
       <c r="L24" s="22"/>
       <c r="M24" s="22"/>
-      <c r="O24" s="37"/>
+      <c r="O24" s="38"/>
       <c r="P24" s="22"/>
       <c r="AC24" s="22"/>
     </row>
     <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" s="39"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="30"/>
       <c r="C25" s="30"/>
       <c r="D25" s="30"/>
@@ -28436,12 +28439,12 @@
       <c r="K25" s="30"/>
       <c r="L25" s="30"/>
       <c r="M25" s="30"/>
-      <c r="O25" s="37"/>
+      <c r="O25" s="38"/>
       <c r="P25" s="30"/>
       <c r="AC25" s="30"/>
     </row>
     <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" s="38"/>
+      <c r="A26" s="39"/>
       <c r="B26" s="22"/>
       <c r="C26" s="22"/>
       <c r="D26" s="22"/>
@@ -28454,12 +28457,12 @@
       <c r="K26" s="22"/>
       <c r="L26" s="22"/>
       <c r="M26" s="22"/>
-      <c r="O26" s="37"/>
+      <c r="O26" s="38"/>
       <c r="P26" s="22"/>
       <c r="AC26" s="22"/>
     </row>
     <row r="27" ht="12.75" customHeight="1">
-      <c r="A27" s="39"/>
+      <c r="A27" s="40"/>
       <c r="B27" s="30"/>
       <c r="C27" s="30"/>
       <c r="D27" s="30"/>
@@ -28472,12 +28475,12 @@
       <c r="K27" s="30"/>
       <c r="L27" s="30"/>
       <c r="M27" s="30"/>
-      <c r="O27" s="37"/>
+      <c r="O27" s="38"/>
       <c r="P27" s="30"/>
       <c r="AC27" s="30"/>
     </row>
     <row r="28" ht="12.75" customHeight="1">
-      <c r="A28" s="38"/>
+      <c r="A28" s="39"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
@@ -28490,12 +28493,12 @@
       <c r="K28" s="22"/>
       <c r="L28" s="22"/>
       <c r="M28" s="22"/>
-      <c r="O28" s="37"/>
+      <c r="O28" s="38"/>
       <c r="P28" s="22"/>
       <c r="AC28" s="22"/>
     </row>
     <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" s="39"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="30"/>
       <c r="C29" s="30"/>
       <c r="D29" s="30"/>
@@ -28508,12 +28511,12 @@
       <c r="K29" s="30"/>
       <c r="L29" s="30"/>
       <c r="M29" s="30"/>
-      <c r="O29" s="37"/>
+      <c r="O29" s="38"/>
       <c r="P29" s="30"/>
       <c r="AC29" s="30"/>
     </row>
     <row r="30" ht="12.75" customHeight="1">
-      <c r="A30" s="38"/>
+      <c r="A30" s="39"/>
       <c r="B30" s="22"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
@@ -28526,12 +28529,12 @@
       <c r="K30" s="22"/>
       <c r="L30" s="22"/>
       <c r="M30" s="22"/>
-      <c r="O30" s="37"/>
+      <c r="O30" s="38"/>
       <c r="P30" s="22"/>
       <c r="AC30" s="22"/>
     </row>
     <row r="31" ht="12.75" customHeight="1">
-      <c r="A31" s="39"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="30"/>
       <c r="C31" s="30"/>
       <c r="D31" s="30"/>
@@ -28544,12 +28547,12 @@
       <c r="K31" s="30"/>
       <c r="L31" s="30"/>
       <c r="M31" s="30"/>
-      <c r="O31" s="37"/>
+      <c r="O31" s="38"/>
       <c r="P31" s="30"/>
       <c r="AC31" s="30"/>
     </row>
     <row r="32" ht="12.75" customHeight="1">
-      <c r="A32" s="38"/>
+      <c r="A32" s="39"/>
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
       <c r="D32" s="22"/>
@@ -28562,12 +28565,12 @@
       <c r="K32" s="22"/>
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
-      <c r="O32" s="37"/>
+      <c r="O32" s="38"/>
       <c r="P32" s="22"/>
       <c r="AC32" s="22"/>
     </row>
     <row r="33" ht="12.75" customHeight="1">
-      <c r="A33" s="39"/>
+      <c r="A33" s="40"/>
       <c r="B33" s="30"/>
       <c r="C33" s="30"/>
       <c r="D33" s="30"/>
@@ -28580,12 +28583,12 @@
       <c r="K33" s="30"/>
       <c r="L33" s="30"/>
       <c r="M33" s="30"/>
-      <c r="O33" s="37"/>
+      <c r="O33" s="38"/>
       <c r="P33" s="30"/>
       <c r="AC33" s="30"/>
     </row>
     <row r="34" ht="12.75" customHeight="1">
-      <c r="A34" s="38"/>
+      <c r="A34" s="39"/>
       <c r="B34" s="22"/>
       <c r="C34" s="22"/>
       <c r="D34" s="22"/>
@@ -28598,12 +28601,12 @@
       <c r="K34" s="22"/>
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
-      <c r="O34" s="37"/>
+      <c r="O34" s="38"/>
       <c r="P34" s="22"/>
       <c r="AC34" s="22"/>
     </row>
     <row r="35" ht="12.75" customHeight="1">
-      <c r="A35" s="39"/>
+      <c r="A35" s="40"/>
       <c r="B35" s="30"/>
       <c r="C35" s="30"/>
       <c r="D35" s="30"/>
@@ -28616,12 +28619,12 @@
       <c r="K35" s="30"/>
       <c r="L35" s="30"/>
       <c r="M35" s="30"/>
-      <c r="O35" s="37"/>
+      <c r="O35" s="38"/>
       <c r="P35" s="30"/>
       <c r="AC35" s="30"/>
     </row>
     <row r="36" ht="12.75" customHeight="1">
-      <c r="A36" s="38"/>
+      <c r="A36" s="39"/>
       <c r="B36" s="22"/>
       <c r="C36" s="22"/>
       <c r="D36" s="22"/>
@@ -28634,12 +28637,12 @@
       <c r="K36" s="22"/>
       <c r="L36" s="22"/>
       <c r="M36" s="22"/>
-      <c r="O36" s="37"/>
+      <c r="O36" s="38"/>
       <c r="P36" s="22"/>
       <c r="AC36" s="22"/>
     </row>
     <row r="37" ht="12.75" customHeight="1">
-      <c r="A37" s="39"/>
+      <c r="A37" s="40"/>
       <c r="B37" s="30"/>
       <c r="C37" s="30"/>
       <c r="D37" s="30"/>
@@ -28652,12 +28655,12 @@
       <c r="K37" s="30"/>
       <c r="L37" s="30"/>
       <c r="M37" s="30"/>
-      <c r="O37" s="37"/>
+      <c r="O37" s="38"/>
       <c r="P37" s="30"/>
       <c r="AC37" s="30"/>
     </row>
     <row r="38" ht="12.75" customHeight="1">
-      <c r="A38" s="38"/>
+      <c r="A38" s="39"/>
       <c r="B38" s="22"/>
       <c r="C38" s="22"/>
       <c r="D38" s="22"/>
@@ -28670,12 +28673,12 @@
       <c r="K38" s="22"/>
       <c r="L38" s="22"/>
       <c r="M38" s="22"/>
-      <c r="O38" s="37"/>
+      <c r="O38" s="38"/>
       <c r="P38" s="22"/>
       <c r="AC38" s="22"/>
     </row>
     <row r="39" ht="12.75" customHeight="1">
-      <c r="A39" s="39"/>
+      <c r="A39" s="40"/>
       <c r="B39" s="30"/>
       <c r="C39" s="30"/>
       <c r="D39" s="30"/>
@@ -28688,12 +28691,12 @@
       <c r="K39" s="30"/>
       <c r="L39" s="30"/>
       <c r="M39" s="30"/>
-      <c r="O39" s="37"/>
+      <c r="O39" s="38"/>
       <c r="P39" s="30"/>
       <c r="AC39" s="30"/>
     </row>
     <row r="40" ht="12.75" customHeight="1">
-      <c r="A40" s="38"/>
+      <c r="A40" s="39"/>
       <c r="B40" s="22"/>
       <c r="C40" s="22"/>
       <c r="D40" s="22"/>
@@ -28706,12 +28709,12 @@
       <c r="K40" s="22"/>
       <c r="L40" s="22"/>
       <c r="M40" s="22"/>
-      <c r="O40" s="37"/>
+      <c r="O40" s="38"/>
       <c r="P40" s="22"/>
       <c r="AC40" s="22"/>
     </row>
     <row r="41" ht="12.75" customHeight="1">
-      <c r="A41" s="39"/>
+      <c r="A41" s="40"/>
       <c r="B41" s="30"/>
       <c r="C41" s="30"/>
       <c r="D41" s="30"/>
@@ -28724,12 +28727,12 @@
       <c r="K41" s="30"/>
       <c r="L41" s="30"/>
       <c r="M41" s="30"/>
-      <c r="O41" s="37"/>
+      <c r="O41" s="38"/>
       <c r="P41" s="30"/>
       <c r="AC41" s="30"/>
     </row>
     <row r="42" ht="12.75" customHeight="1">
-      <c r="A42" s="38"/>
+      <c r="A42" s="39"/>
       <c r="B42" s="22"/>
       <c r="C42" s="22"/>
       <c r="D42" s="22"/>
@@ -28742,12 +28745,12 @@
       <c r="K42" s="22"/>
       <c r="L42" s="22"/>
       <c r="M42" s="22"/>
-      <c r="O42" s="37"/>
+      <c r="O42" s="38"/>
       <c r="P42" s="22"/>
       <c r="AC42" s="22"/>
     </row>
     <row r="43" ht="12.75" customHeight="1">
-      <c r="A43" s="39"/>
+      <c r="A43" s="40"/>
       <c r="B43" s="30"/>
       <c r="C43" s="30"/>
       <c r="D43" s="30"/>
@@ -28760,12 +28763,12 @@
       <c r="K43" s="30"/>
       <c r="L43" s="30"/>
       <c r="M43" s="30"/>
-      <c r="O43" s="37"/>
+      <c r="O43" s="38"/>
       <c r="P43" s="30"/>
       <c r="AC43" s="30"/>
     </row>
     <row r="44" ht="12.75" customHeight="1">
-      <c r="A44" s="38"/>
+      <c r="A44" s="39"/>
       <c r="B44" s="22"/>
       <c r="C44" s="22"/>
       <c r="D44" s="22"/>
@@ -28778,12 +28781,12 @@
       <c r="K44" s="22"/>
       <c r="L44" s="22"/>
       <c r="M44" s="22"/>
-      <c r="O44" s="37"/>
+      <c r="O44" s="38"/>
       <c r="P44" s="22"/>
       <c r="AC44" s="22"/>
     </row>
     <row r="45" ht="12.75" customHeight="1">
-      <c r="A45" s="39"/>
+      <c r="A45" s="40"/>
       <c r="B45" s="30"/>
       <c r="C45" s="30"/>
       <c r="D45" s="30"/>
@@ -28796,12 +28799,12 @@
       <c r="K45" s="30"/>
       <c r="L45" s="30"/>
       <c r="M45" s="30"/>
-      <c r="O45" s="37"/>
+      <c r="O45" s="38"/>
       <c r="P45" s="30"/>
       <c r="AC45" s="30"/>
     </row>
     <row r="46" ht="12.75" customHeight="1">
-      <c r="A46" s="38"/>
+      <c r="A46" s="39"/>
       <c r="B46" s="22"/>
       <c r="C46" s="22"/>
       <c r="D46" s="22"/>
@@ -28814,12 +28817,12 @@
       <c r="K46" s="22"/>
       <c r="L46" s="22"/>
       <c r="M46" s="22"/>
-      <c r="O46" s="37"/>
+      <c r="O46" s="38"/>
       <c r="P46" s="22"/>
       <c r="AC46" s="22"/>
     </row>
     <row r="47" ht="12.75" customHeight="1">
-      <c r="A47" s="39"/>
+      <c r="A47" s="40"/>
       <c r="B47" s="30"/>
       <c r="C47" s="30"/>
       <c r="D47" s="30"/>
@@ -28832,12 +28835,12 @@
       <c r="K47" s="30"/>
       <c r="L47" s="30"/>
       <c r="M47" s="30"/>
-      <c r="O47" s="37"/>
+      <c r="O47" s="38"/>
       <c r="P47" s="30"/>
       <c r="AC47" s="30"/>
     </row>
     <row r="48" ht="12.75" customHeight="1">
-      <c r="A48" s="38"/>
+      <c r="A48" s="39"/>
       <c r="B48" s="22"/>
       <c r="C48" s="22"/>
       <c r="D48" s="22"/>
@@ -28850,12 +28853,12 @@
       <c r="K48" s="22"/>
       <c r="L48" s="22"/>
       <c r="M48" s="22"/>
-      <c r="O48" s="37"/>
+      <c r="O48" s="38"/>
       <c r="P48" s="22"/>
       <c r="AC48" s="22"/>
     </row>
     <row r="49" ht="12.75" customHeight="1">
-      <c r="A49" s="39"/>
+      <c r="A49" s="40"/>
       <c r="B49" s="30"/>
       <c r="C49" s="30"/>
       <c r="D49" s="30"/>
@@ -28868,12 +28871,12 @@
       <c r="K49" s="30"/>
       <c r="L49" s="30"/>
       <c r="M49" s="30"/>
-      <c r="O49" s="37"/>
+      <c r="O49" s="38"/>
       <c r="P49" s="30"/>
       <c r="AC49" s="30"/>
     </row>
     <row r="50" ht="12.75" customHeight="1">
-      <c r="A50" s="38"/>
+      <c r="A50" s="39"/>
       <c r="B50" s="22"/>
       <c r="C50" s="22"/>
       <c r="D50" s="22"/>
@@ -28886,12 +28889,12 @@
       <c r="K50" s="22"/>
       <c r="L50" s="22"/>
       <c r="M50" s="22"/>
-      <c r="O50" s="37"/>
+      <c r="O50" s="38"/>
       <c r="P50" s="22"/>
       <c r="AC50" s="22"/>
     </row>
     <row r="51" ht="12.75" customHeight="1">
-      <c r="A51" s="39"/>
+      <c r="A51" s="40"/>
       <c r="B51" s="30"/>
       <c r="C51" s="30"/>
       <c r="D51" s="30"/>
@@ -28904,12 +28907,12 @@
       <c r="K51" s="30"/>
       <c r="L51" s="30"/>
       <c r="M51" s="30"/>
-      <c r="O51" s="37"/>
+      <c r="O51" s="38"/>
       <c r="P51" s="30"/>
       <c r="AC51" s="30"/>
     </row>
     <row r="52" ht="12.75" customHeight="1">
-      <c r="A52" s="38"/>
+      <c r="A52" s="39"/>
       <c r="B52" s="22"/>
       <c r="C52" s="22"/>
       <c r="D52" s="22"/>
@@ -28922,12 +28925,12 @@
       <c r="K52" s="22"/>
       <c r="L52" s="22"/>
       <c r="M52" s="22"/>
-      <c r="O52" s="37"/>
+      <c r="O52" s="38"/>
       <c r="P52" s="22"/>
       <c r="AC52" s="22"/>
     </row>
     <row r="53" ht="12.75" customHeight="1">
-      <c r="A53" s="39"/>
+      <c r="A53" s="40"/>
       <c r="B53" s="30"/>
       <c r="C53" s="30"/>
       <c r="D53" s="30"/>
@@ -28940,12 +28943,12 @@
       <c r="K53" s="30"/>
       <c r="L53" s="30"/>
       <c r="M53" s="30"/>
-      <c r="O53" s="37"/>
+      <c r="O53" s="38"/>
       <c r="P53" s="30"/>
       <c r="AC53" s="30"/>
     </row>
     <row r="54" ht="12.75" customHeight="1">
-      <c r="A54" s="38"/>
+      <c r="A54" s="39"/>
       <c r="B54" s="22"/>
       <c r="C54" s="22"/>
       <c r="D54" s="22"/>
@@ -28958,12 +28961,12 @@
       <c r="K54" s="22"/>
       <c r="L54" s="22"/>
       <c r="M54" s="22"/>
-      <c r="O54" s="37"/>
+      <c r="O54" s="38"/>
       <c r="P54" s="22"/>
       <c r="AC54" s="22"/>
     </row>
     <row r="55" ht="12.75" customHeight="1">
-      <c r="A55" s="39"/>
+      <c r="A55" s="40"/>
       <c r="B55" s="30"/>
       <c r="C55" s="30"/>
       <c r="D55" s="30"/>
@@ -28976,12 +28979,12 @@
       <c r="K55" s="30"/>
       <c r="L55" s="30"/>
       <c r="M55" s="30"/>
-      <c r="O55" s="37"/>
+      <c r="O55" s="38"/>
       <c r="P55" s="30"/>
       <c r="AC55" s="30"/>
     </row>
     <row r="56" ht="12.75" customHeight="1">
-      <c r="A56" s="38"/>
+      <c r="A56" s="39"/>
       <c r="B56" s="22"/>
       <c r="C56" s="22"/>
       <c r="D56" s="22"/>
@@ -28994,12 +28997,12 @@
       <c r="K56" s="22"/>
       <c r="L56" s="22"/>
       <c r="M56" s="22"/>
-      <c r="O56" s="37"/>
+      <c r="O56" s="38"/>
       <c r="P56" s="22"/>
       <c r="AC56" s="22"/>
     </row>
     <row r="57" ht="12.75" customHeight="1">
-      <c r="A57" s="39"/>
+      <c r="A57" s="40"/>
       <c r="B57" s="30"/>
       <c r="C57" s="30"/>
       <c r="D57" s="30"/>
@@ -29012,12 +29015,12 @@
       <c r="K57" s="30"/>
       <c r="L57" s="30"/>
       <c r="M57" s="30"/>
-      <c r="O57" s="37"/>
+      <c r="O57" s="38"/>
       <c r="P57" s="30"/>
       <c r="AC57" s="30"/>
     </row>
     <row r="58" ht="12.75" customHeight="1">
-      <c r="A58" s="38"/>
+      <c r="A58" s="39"/>
       <c r="B58" s="22"/>
       <c r="C58" s="22"/>
       <c r="D58" s="22"/>
@@ -29030,12 +29033,12 @@
       <c r="K58" s="22"/>
       <c r="L58" s="22"/>
       <c r="M58" s="22"/>
-      <c r="O58" s="37"/>
+      <c r="O58" s="38"/>
       <c r="P58" s="22"/>
       <c r="AC58" s="22"/>
     </row>
     <row r="59" ht="12.75" customHeight="1">
-      <c r="A59" s="39"/>
+      <c r="A59" s="40"/>
       <c r="B59" s="30"/>
       <c r="C59" s="30"/>
       <c r="D59" s="30"/>
@@ -29048,12 +29051,12 @@
       <c r="K59" s="30"/>
       <c r="L59" s="30"/>
       <c r="M59" s="30"/>
-      <c r="O59" s="37"/>
+      <c r="O59" s="38"/>
       <c r="P59" s="30"/>
       <c r="AC59" s="30"/>
     </row>
     <row r="60" ht="12.75" customHeight="1">
-      <c r="A60" s="38"/>
+      <c r="A60" s="39"/>
       <c r="B60" s="22"/>
       <c r="C60" s="22"/>
       <c r="D60" s="22"/>
@@ -29066,12 +29069,12 @@
       <c r="K60" s="22"/>
       <c r="L60" s="22"/>
       <c r="M60" s="22"/>
-      <c r="O60" s="37"/>
+      <c r="O60" s="38"/>
       <c r="P60" s="22"/>
       <c r="AC60" s="22"/>
     </row>
     <row r="61" ht="12.75" customHeight="1">
-      <c r="A61" s="39"/>
+      <c r="A61" s="40"/>
       <c r="B61" s="30"/>
       <c r="C61" s="30"/>
       <c r="D61" s="30"/>
@@ -29084,12 +29087,12 @@
       <c r="K61" s="30"/>
       <c r="L61" s="30"/>
       <c r="M61" s="30"/>
-      <c r="O61" s="37"/>
+      <c r="O61" s="38"/>
       <c r="P61" s="30"/>
       <c r="AC61" s="30"/>
     </row>
     <row r="62" ht="12.75" customHeight="1">
-      <c r="A62" s="38"/>
+      <c r="A62" s="39"/>
       <c r="B62" s="22"/>
       <c r="C62" s="22"/>
       <c r="D62" s="22"/>
@@ -29102,12 +29105,12 @@
       <c r="K62" s="22"/>
       <c r="L62" s="22"/>
       <c r="M62" s="22"/>
-      <c r="O62" s="37"/>
+      <c r="O62" s="38"/>
       <c r="P62" s="22"/>
       <c r="AC62" s="22"/>
     </row>
     <row r="63" ht="12.75" customHeight="1">
-      <c r="A63" s="39"/>
+      <c r="A63" s="40"/>
       <c r="B63" s="30"/>
       <c r="C63" s="30"/>
       <c r="D63" s="30"/>
@@ -29120,12 +29123,12 @@
       <c r="K63" s="30"/>
       <c r="L63" s="30"/>
       <c r="M63" s="30"/>
-      <c r="O63" s="37"/>
+      <c r="O63" s="38"/>
       <c r="P63" s="30"/>
       <c r="AC63" s="30"/>
     </row>
     <row r="64" ht="12.75" customHeight="1">
-      <c r="A64" s="38"/>
+      <c r="A64" s="39"/>
       <c r="B64" s="22"/>
       <c r="C64" s="22"/>
       <c r="D64" s="22"/>
@@ -29138,12 +29141,12 @@
       <c r="K64" s="22"/>
       <c r="L64" s="22"/>
       <c r="M64" s="22"/>
-      <c r="O64" s="37"/>
+      <c r="O64" s="38"/>
       <c r="P64" s="22"/>
       <c r="AC64" s="22"/>
     </row>
     <row r="65" ht="12.75" customHeight="1">
-      <c r="A65" s="39"/>
+      <c r="A65" s="40"/>
       <c r="B65" s="30"/>
       <c r="C65" s="30"/>
       <c r="D65" s="30"/>
@@ -29156,12 +29159,12 @@
       <c r="K65" s="30"/>
       <c r="L65" s="30"/>
       <c r="M65" s="30"/>
-      <c r="O65" s="37"/>
+      <c r="O65" s="38"/>
       <c r="P65" s="30"/>
       <c r="AC65" s="30"/>
     </row>
     <row r="66" ht="12.75" customHeight="1">
-      <c r="A66" s="38"/>
+      <c r="A66" s="39"/>
       <c r="B66" s="22"/>
       <c r="C66" s="22"/>
       <c r="D66" s="22"/>
@@ -29174,12 +29177,12 @@
       <c r="K66" s="22"/>
       <c r="L66" s="22"/>
       <c r="M66" s="22"/>
-      <c r="O66" s="37"/>
+      <c r="O66" s="38"/>
       <c r="P66" s="22"/>
       <c r="AC66" s="22"/>
     </row>
     <row r="67" ht="12.75" customHeight="1">
-      <c r="A67" s="39"/>
+      <c r="A67" s="40"/>
       <c r="B67" s="30"/>
       <c r="C67" s="30"/>
       <c r="D67" s="30"/>
@@ -29192,12 +29195,12 @@
       <c r="K67" s="30"/>
       <c r="L67" s="30"/>
       <c r="M67" s="30"/>
-      <c r="O67" s="37"/>
+      <c r="O67" s="38"/>
       <c r="P67" s="30"/>
       <c r="AC67" s="30"/>
     </row>
     <row r="68" ht="12.75" customHeight="1">
-      <c r="A68" s="38"/>
+      <c r="A68" s="39"/>
       <c r="B68" s="22"/>
       <c r="C68" s="22"/>
       <c r="D68" s="22"/>
@@ -29210,12 +29213,12 @@
       <c r="K68" s="22"/>
       <c r="L68" s="22"/>
       <c r="M68" s="22"/>
-      <c r="O68" s="37"/>
+      <c r="O68" s="38"/>
       <c r="P68" s="22"/>
       <c r="AC68" s="22"/>
     </row>
     <row r="69" ht="12.75" customHeight="1">
-      <c r="A69" s="39"/>
+      <c r="A69" s="40"/>
       <c r="B69" s="30"/>
       <c r="C69" s="30"/>
       <c r="D69" s="30"/>
@@ -29228,12 +29231,12 @@
       <c r="K69" s="30"/>
       <c r="L69" s="30"/>
       <c r="M69" s="30"/>
-      <c r="O69" s="37"/>
+      <c r="O69" s="38"/>
       <c r="P69" s="30"/>
       <c r="AC69" s="30"/>
     </row>
     <row r="70" ht="12.75" customHeight="1">
-      <c r="A70" s="38"/>
+      <c r="A70" s="39"/>
       <c r="B70" s="22"/>
       <c r="C70" s="22"/>
       <c r="D70" s="22"/>
@@ -29246,12 +29249,12 @@
       <c r="K70" s="22"/>
       <c r="L70" s="22"/>
       <c r="M70" s="22"/>
-      <c r="O70" s="37"/>
+      <c r="O70" s="38"/>
       <c r="P70" s="22"/>
       <c r="AC70" s="22"/>
     </row>
     <row r="71" ht="12.75" customHeight="1">
-      <c r="A71" s="39"/>
+      <c r="A71" s="40"/>
       <c r="B71" s="30"/>
       <c r="C71" s="30"/>
       <c r="D71" s="30"/>
@@ -29264,12 +29267,12 @@
       <c r="K71" s="30"/>
       <c r="L71" s="30"/>
       <c r="M71" s="30"/>
-      <c r="O71" s="37"/>
+      <c r="O71" s="38"/>
       <c r="P71" s="30"/>
       <c r="AC71" s="30"/>
     </row>
     <row r="72" ht="12.75" customHeight="1">
-      <c r="A72" s="38"/>
+      <c r="A72" s="39"/>
       <c r="B72" s="22"/>
       <c r="C72" s="22"/>
       <c r="D72" s="22"/>
@@ -29282,12 +29285,12 @@
       <c r="K72" s="22"/>
       <c r="L72" s="22"/>
       <c r="M72" s="22"/>
-      <c r="O72" s="37"/>
+      <c r="O72" s="38"/>
       <c r="P72" s="22"/>
       <c r="AC72" s="22"/>
     </row>
     <row r="73" ht="12.75" customHeight="1">
-      <c r="A73" s="39"/>
+      <c r="A73" s="40"/>
       <c r="B73" s="30"/>
       <c r="C73" s="30"/>
       <c r="D73" s="30"/>
@@ -29300,12 +29303,12 @@
       <c r="K73" s="30"/>
       <c r="L73" s="30"/>
       <c r="M73" s="30"/>
-      <c r="O73" s="37"/>
+      <c r="O73" s="38"/>
       <c r="P73" s="30"/>
       <c r="AC73" s="30"/>
     </row>
     <row r="74" ht="12.75" customHeight="1">
-      <c r="A74" s="38"/>
+      <c r="A74" s="39"/>
       <c r="B74" s="22"/>
       <c r="C74" s="22"/>
       <c r="D74" s="22"/>
@@ -29318,12 +29321,12 @@
       <c r="K74" s="22"/>
       <c r="L74" s="22"/>
       <c r="M74" s="22"/>
-      <c r="O74" s="37"/>
+      <c r="O74" s="38"/>
       <c r="P74" s="22"/>
       <c r="AC74" s="22"/>
     </row>
     <row r="75" ht="12.75" customHeight="1">
-      <c r="A75" s="39"/>
+      <c r="A75" s="40"/>
       <c r="B75" s="30"/>
       <c r="C75" s="30"/>
       <c r="D75" s="30"/>
@@ -29336,7 +29339,7 @@
       <c r="K75" s="30"/>
       <c r="L75" s="30"/>
       <c r="M75" s="30"/>
-      <c r="O75" s="37"/>
+      <c r="O75" s="38"/>
       <c r="P75" s="30"/>
       <c r="AC75" s="30"/>
     </row>
@@ -32900,22 +32903,22 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="41">
+      <c r="C2" s="42">
         <v>2.101184477E7</v>
       </c>
-      <c r="D2" s="42">
+      <c r="D2" s="43">
         <v>44008.0</v>
       </c>
       <c r="E2" s="36">
         <v>75.0</v>
       </c>
-      <c r="F2" s="41">
+      <c r="F2" s="42">
         <v>2.101184477E7</v>
       </c>
       <c r="G2" s="8">
@@ -32924,12 +32927,12 @@
       <c r="H2" s="8">
         <v>44012.0</v>
       </c>
-      <c r="I2" s="41">
+      <c r="I2" s="42">
         <v>2.101184477E7</v>
       </c>
       <c r="J2" s="13"/>
       <c r="K2" s="13"/>
-      <c r="L2" s="43">
+      <c r="L2" s="44">
         <v>1.0505922385E7</v>
       </c>
       <c r="M2" s="13"/>
@@ -32942,22 +32945,22 @@
       <c r="R2" s="13"/>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="45">
+      <c r="C3" s="46">
         <v>1.578213759E7</v>
       </c>
-      <c r="D3" s="46">
+      <c r="D3" s="47">
         <v>44008.0</v>
       </c>
       <c r="E3" s="36">
         <v>75.0</v>
       </c>
-      <c r="F3" s="45">
+      <c r="F3" s="46">
         <v>1.578213759E7</v>
       </c>
       <c r="G3" s="8">
@@ -32966,12 +32969,12 @@
       <c r="H3" s="8">
         <v>44012.0</v>
       </c>
-      <c r="I3" s="45">
+      <c r="I3" s="46">
         <v>1.578213759E7</v>
       </c>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
-      <c r="L3" s="43">
+      <c r="L3" s="44">
         <v>1.578213759E7</v>
       </c>
       <c r="M3" s="13"/>
@@ -32982,22 +32985,22 @@
       <c r="R3" s="13"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4" s="42">
         <v>9647704.77</v>
       </c>
-      <c r="D4" s="42">
+      <c r="D4" s="43">
         <v>44008.0</v>
       </c>
       <c r="E4" s="36">
         <v>75.0</v>
       </c>
-      <c r="F4" s="41">
+      <c r="F4" s="42">
         <v>9647704.77</v>
       </c>
       <c r="G4" s="8">
@@ -33006,12 +33009,12 @@
       <c r="H4" s="8">
         <v>44012.0</v>
       </c>
-      <c r="I4" s="41">
+      <c r="I4" s="42">
         <v>9647704.77</v>
       </c>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="43">
+      <c r="L4" s="44">
         <v>4823852.385</v>
       </c>
       <c r="M4" s="13"/>
@@ -33020,7 +33023,7 @@
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
       <c r="R4" s="13"/>
-      <c r="T4" s="43">
+      <c r="T4" s="44">
         <v>4823852.385</v>
       </c>
     </row>
@@ -33061,7 +33064,7 @@
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="K10" s="13"/>
-      <c r="M10" s="47"/>
+      <c r="M10" s="48"/>
       <c r="O10" s="13"/>
       <c r="Q10" s="13"/>
       <c r="R10" s="13"/>

</xml_diff>

<commit_message>
add cumulative validation for direct tab
</commit_message>
<xml_diff>
--- a/tests/server/fixtures/file-success/EOHHS-075-12312020-simple-v1.xlsx
+++ b/tests/server/fixtures/file-success/EOHHS-075-12312020-simple-v1.xlsx
@@ -1318,7 +1318,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1407,6 +1407,9 @@
     <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="10" fillId="0" fontId="4" numFmtId="3" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="10" fillId="0" fontId="4" numFmtId="14" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="9" fillId="9" fontId="4" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="10" fillId="0" fontId="4" numFmtId="4" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
@@ -7999,10 +8002,10 @@
       <c r="C3" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D3" s="49">
+      <c r="D3" s="50">
         <v>2163121.97</v>
       </c>
-      <c r="E3" s="49">
+      <c r="E3" s="50">
         <v>840542.45</v>
       </c>
     </row>
@@ -8016,10 +8019,10 @@
       <c r="C4" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D4" s="49">
+      <c r="D4" s="50">
         <v>5957909.0</v>
       </c>
-      <c r="E4" s="49">
+      <c r="E4" s="50">
         <v>5957909.0</v>
       </c>
     </row>
@@ -10104,119 +10107,119 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>222</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="51" t="s">
         <v>223</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="51" t="s">
         <v>224</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="51" t="s">
         <v>224</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="51" t="s">
         <v>214</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="51" t="s">
         <v>224</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="H1" s="51" t="s">
         <v>225</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="51" t="s">
         <v>215</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="J1" s="51" t="s">
         <v>215</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="K1" s="51" t="s">
         <v>217</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="L1" s="51" t="s">
         <v>226</v>
       </c>
-      <c r="M1" s="50" t="s">
+      <c r="M1" s="51" t="s">
         <v>226</v>
       </c>
-      <c r="N1" s="50" t="s">
+      <c r="N1" s="51" t="s">
         <v>227</v>
       </c>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="50"/>
-      <c r="V1" s="50"/>
-      <c r="W1" s="50"/>
-      <c r="X1" s="50"/>
-      <c r="Y1" s="50"/>
-      <c r="Z1" s="50"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="51"/>
+      <c r="Z1" s="51"/>
     </row>
     <row r="2" ht="15.0" customHeight="1">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="51" t="s">
         <v>228</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="52" t="s">
         <v>229</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="G2" s="51" t="s">
+      <c r="G2" s="52" t="s">
         <v>230</v>
       </c>
-      <c r="H2" s="51" t="s">
+      <c r="H2" s="52" t="s">
         <v>231</v>
       </c>
-      <c r="I2" s="51" t="s">
+      <c r="I2" s="52" t="s">
         <v>170</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="J2" s="52" t="s">
         <v>232</v>
       </c>
-      <c r="K2" s="51" t="s">
+      <c r="K2" s="52" t="s">
         <v>194</v>
       </c>
-      <c r="L2" s="51" t="s">
+      <c r="L2" s="52" t="s">
         <v>211</v>
       </c>
-      <c r="M2" s="51" t="s">
+      <c r="M2" s="52" t="s">
         <v>212</v>
       </c>
-      <c r="N2" s="51" t="s">
+      <c r="N2" s="52" t="s">
         <v>212</v>
       </c>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="50"/>
-      <c r="V2" s="50"/>
-      <c r="W2" s="50"/>
-      <c r="X2" s="50"/>
-      <c r="Y2" s="50"/>
-      <c r="Z2" s="50"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="51"/>
+      <c r="V2" s="51"/>
+      <c r="W2" s="51"/>
+      <c r="X2" s="51"/>
+      <c r="Y2" s="51"/>
+      <c r="Z2" s="51"/>
     </row>
     <row r="3" ht="15.0" customHeight="1">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="51" t="s">
         <v>233</v>
       </c>
       <c r="B3" s="18" t="s">
@@ -10316,7 +10319,7 @@
       <c r="F5" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="G5" s="52" t="s">
+      <c r="G5" s="53" t="s">
         <v>251</v>
       </c>
       <c r="L5" s="18" t="s">
@@ -10358,7 +10361,7 @@
       <c r="D8" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="E8" s="53" t="s">
+      <c r="E8" s="54" t="s">
         <v>259</v>
       </c>
     </row>
@@ -11647,102 +11650,102 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="2" ht="15.0" customHeight="1">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="55" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="1">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="55" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="4" ht="15.0" customHeight="1">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="55" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" ht="15.0" customHeight="1">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="55" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="1">
-      <c r="A7" s="50"/>
-      <c r="B7" s="50" t="s">
+      <c r="A7" s="51"/>
+      <c r="B7" s="51" t="s">
         <v>325</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50" t="s">
+      <c r="C7" s="51"/>
+      <c r="D7" s="51" t="s">
         <v>326</v>
       </c>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50" t="s">
+      <c r="E7" s="51"/>
+      <c r="F7" s="51" t="s">
         <v>327</v>
       </c>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="50"/>
-      <c r="P7" s="50"/>
-      <c r="Q7" s="50"/>
-      <c r="R7" s="50"/>
-      <c r="S7" s="50"/>
-      <c r="T7" s="50"/>
-      <c r="U7" s="50"/>
-      <c r="V7" s="50"/>
-      <c r="W7" s="50"/>
-      <c r="X7" s="50"/>
-      <c r="Y7" s="50"/>
-      <c r="Z7" s="50"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="51"/>
+      <c r="P7" s="51"/>
+      <c r="Q7" s="51"/>
+      <c r="R7" s="51"/>
+      <c r="S7" s="51"/>
+      <c r="T7" s="51"/>
+      <c r="U7" s="51"/>
+      <c r="V7" s="51"/>
+      <c r="W7" s="51"/>
+      <c r="X7" s="51"/>
+      <c r="Y7" s="51"/>
+      <c r="Z7" s="51"/>
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="18" t="s">
         <v>328</v>
       </c>
-      <c r="B8" s="55"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="56"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="57"/>
     </row>
     <row r="9" ht="15.0" customHeight="1">
       <c r="A9" s="18" t="s">
         <v>329</v>
       </c>
-      <c r="B9" s="55"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="56"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="57"/>
     </row>
     <row r="10" ht="15.0" customHeight="1">
       <c r="A10" s="18" t="s">
         <v>330</v>
       </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="55">
+      <c r="B10" s="57"/>
+      <c r="C10" s="56">
         <f>B8+B9</f>
         <v>0</v>
       </c>
-      <c r="D10" s="56"/>
-      <c r="E10" s="55">
+      <c r="D10" s="57"/>
+      <c r="E10" s="56">
         <f>D8+D9</f>
         <v>0</v>
       </c>
-      <c r="F10" s="56"/>
-      <c r="G10" s="55">
+      <c r="F10" s="57"/>
+      <c r="G10" s="56">
         <f>F8+F9</f>
         <v>0</v>
       </c>
@@ -11751,40 +11754,40 @@
       <c r="A11" s="18" t="s">
         <v>331</v>
       </c>
-      <c r="B11" s="55"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="56"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="57"/>
     </row>
     <row r="12" ht="15.0" customHeight="1">
       <c r="A12" s="18" t="s">
         <v>332</v>
       </c>
-      <c r="B12" s="55"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="56"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="57"/>
     </row>
     <row r="13" ht="15.0" customHeight="1">
       <c r="A13" s="18" t="s">
         <v>333</v>
       </c>
-      <c r="B13" s="56"/>
-      <c r="C13" s="55">
+      <c r="B13" s="57"/>
+      <c r="C13" s="56">
         <f>B11+B12</f>
         <v>0</v>
       </c>
-      <c r="D13" s="56"/>
-      <c r="E13" s="55">
+      <c r="D13" s="57"/>
+      <c r="E13" s="56">
         <f>D11+D12</f>
         <v>0</v>
       </c>
-      <c r="F13" s="56"/>
-      <c r="G13" s="55">
+      <c r="F13" s="57"/>
+      <c r="G13" s="56">
         <f>F11+F12</f>
         <v>0</v>
       </c>
@@ -11793,40 +11796,40 @@
       <c r="A14" s="18" t="s">
         <v>334</v>
       </c>
-      <c r="B14" s="55"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="56"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="57"/>
     </row>
     <row r="15" ht="15.0" customHeight="1">
       <c r="A15" s="18" t="s">
         <v>335</v>
       </c>
-      <c r="B15" s="55"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="56"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="57"/>
     </row>
     <row r="16" ht="15.0" customHeight="1">
       <c r="A16" s="18" t="s">
         <v>336</v>
       </c>
-      <c r="B16" s="56"/>
-      <c r="C16" s="55">
+      <c r="B16" s="57"/>
+      <c r="C16" s="56">
         <f>B14+B15</f>
         <v>0</v>
       </c>
-      <c r="D16" s="56"/>
-      <c r="E16" s="55">
+      <c r="D16" s="57"/>
+      <c r="E16" s="56">
         <f>D14+D15</f>
         <v>0</v>
       </c>
-      <c r="F16" s="56"/>
-      <c r="G16" s="55">
+      <c r="F16" s="57"/>
+      <c r="G16" s="56">
         <f>F14+F15</f>
         <v>0</v>
       </c>
@@ -11835,40 +11838,40 @@
       <c r="A17" s="18" t="s">
         <v>337</v>
       </c>
-      <c r="B17" s="55"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="56"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="57"/>
     </row>
     <row r="18" ht="15.0" customHeight="1">
       <c r="A18" s="18" t="s">
         <v>338</v>
       </c>
-      <c r="B18" s="55"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="56"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="57"/>
     </row>
     <row r="19" ht="15.0" customHeight="1">
       <c r="A19" s="18" t="s">
         <v>339</v>
       </c>
-      <c r="B19" s="56"/>
-      <c r="C19" s="55">
+      <c r="B19" s="57"/>
+      <c r="C19" s="56">
         <f>B17+B18</f>
         <v>0</v>
       </c>
-      <c r="D19" s="56"/>
-      <c r="E19" s="55">
+      <c r="D19" s="57"/>
+      <c r="E19" s="56">
         <f>D17+D18</f>
         <v>0</v>
       </c>
-      <c r="F19" s="56"/>
-      <c r="G19" s="55">
+      <c r="F19" s="57"/>
+      <c r="G19" s="56">
         <f>F17+F18</f>
         <v>0</v>
       </c>
@@ -11877,40 +11880,40 @@
       <c r="A20" s="18" t="s">
         <v>340</v>
       </c>
-      <c r="B20" s="55"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="56"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="57"/>
     </row>
     <row r="21" ht="15.0" customHeight="1">
       <c r="A21" s="18" t="s">
         <v>341</v>
       </c>
-      <c r="B21" s="55"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="56"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="57"/>
     </row>
     <row r="22" ht="15.0" customHeight="1">
       <c r="A22" s="18" t="s">
         <v>342</v>
       </c>
-      <c r="B22" s="56"/>
-      <c r="C22" s="55">
+      <c r="B22" s="57"/>
+      <c r="C22" s="56">
         <f>B20+B21</f>
         <v>0</v>
       </c>
-      <c r="D22" s="56"/>
-      <c r="E22" s="55">
+      <c r="D22" s="57"/>
+      <c r="E22" s="56">
         <f>D20+D21</f>
         <v>0</v>
       </c>
-      <c r="F22" s="56"/>
-      <c r="G22" s="55">
+      <c r="F22" s="57"/>
+      <c r="G22" s="56">
         <f>F20+F21</f>
         <v>0</v>
       </c>
@@ -11919,51 +11922,51 @@
       <c r="A23" s="18" t="s">
         <v>343</v>
       </c>
-      <c r="B23" s="56"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="55"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="56"/>
     </row>
     <row r="24" ht="15.0" customHeight="1">
-      <c r="A24" s="50" t="s">
+      <c r="A24" s="51" t="s">
         <v>344</v>
       </c>
-      <c r="B24" s="57"/>
-      <c r="C24" s="57">
+      <c r="B24" s="58"/>
+      <c r="C24" s="58">
         <f>C10+C13+C16+C19+C22</f>
         <v>0</v>
       </c>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57">
+      <c r="D24" s="58"/>
+      <c r="E24" s="58">
         <f>E10+E13+E16+E19+E22</f>
         <v>0</v>
       </c>
-      <c r="F24" s="57"/>
-      <c r="G24" s="57">
+      <c r="F24" s="58"/>
+      <c r="G24" s="58">
         <f>G10+G13+G16+G19+G22</f>
         <v>0</v>
       </c>
-      <c r="H24" s="50"/>
-      <c r="I24" s="50"/>
-      <c r="J24" s="50"/>
-      <c r="K24" s="50"/>
-      <c r="L24" s="50"/>
-      <c r="M24" s="50"/>
-      <c r="N24" s="50"/>
-      <c r="O24" s="50"/>
-      <c r="P24" s="50"/>
-      <c r="Q24" s="50"/>
-      <c r="R24" s="50"/>
-      <c r="S24" s="50"/>
-      <c r="T24" s="50"/>
-      <c r="U24" s="50"/>
-      <c r="V24" s="50"/>
-      <c r="W24" s="50"/>
-      <c r="X24" s="50"/>
-      <c r="Y24" s="50"/>
-      <c r="Z24" s="50"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="51"/>
+      <c r="L24" s="51"/>
+      <c r="M24" s="51"/>
+      <c r="N24" s="51"/>
+      <c r="O24" s="51"/>
+      <c r="P24" s="51"/>
+      <c r="Q24" s="51"/>
+      <c r="R24" s="51"/>
+      <c r="S24" s="51"/>
+      <c r="T24" s="51"/>
+      <c r="U24" s="51"/>
+      <c r="V24" s="51"/>
+      <c r="W24" s="51"/>
+      <c r="X24" s="51"/>
+      <c r="Y24" s="51"/>
+      <c r="Z24" s="51"/>
     </row>
     <row r="25" ht="15.75" customHeight="1"/>
     <row r="26" ht="15.75" customHeight="1"/>
@@ -32991,8 +32994,8 @@
       <c r="B4" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="42">
-        <v>9647704.77</v>
+      <c r="C4" s="48">
+        <v>1.0964770477E8</v>
       </c>
       <c r="D4" s="43">
         <v>44008.0</v>
@@ -33064,7 +33067,7 @@
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="K10" s="13"/>
-      <c r="M10" s="48"/>
+      <c r="M10" s="49"/>
       <c r="O10" s="13"/>
       <c r="Q10" s="13"/>
       <c r="R10" s="13"/>

</xml_diff>

<commit_message>
add cumulative validation for grants
</commit_message>
<xml_diff>
--- a/tests/server/fixtures/file-success/EOHHS-075-12312020-simple-v1.xlsx
+++ b/tests/server/fixtures/file-success/EOHHS-075-12312020-simple-v1.xlsx
@@ -23178,8 +23178,8 @@
       <c r="D2" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="E2" s="37">
-        <v>2927600.0</v>
+      <c r="E2" s="23">
+        <v>1.29276E7</v>
       </c>
       <c r="F2" s="24">
         <v>43969.64884259259</v>

</xml_diff>

<commit_message>
add cumulative validations for loans
</commit_message>
<xml_diff>
--- a/tests/server/fixtures/file-success/EOHHS-075-12312020-simple-v1.xlsx
+++ b/tests/server/fixtures/file-success/EOHHS-075-12312020-simple-v1.xlsx
@@ -1318,7 +1318,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1400,6 +1400,9 @@
     <xf borderId="1" fillId="8" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="7" fillId="8" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="9" fillId="9" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="9" fillId="9" fontId="4" numFmtId="3" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="9" fillId="9" fontId="4" numFmtId="14" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
@@ -8002,10 +8005,10 @@
       <c r="C3" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D3" s="50">
+      <c r="D3" s="51">
         <v>2163121.97</v>
       </c>
-      <c r="E3" s="50">
+      <c r="E3" s="51">
         <v>840542.45</v>
       </c>
     </row>
@@ -8019,10 +8022,10 @@
       <c r="C4" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D4" s="50">
+      <c r="D4" s="51">
         <v>5957909.0</v>
       </c>
-      <c r="E4" s="50">
+      <c r="E4" s="51">
         <v>5957909.0</v>
       </c>
     </row>
@@ -9077,10 +9080,10 @@
       <c r="B2" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C2" s="44">
+      <c r="C2" s="45">
         <v>1567999.5</v>
       </c>
-      <c r="D2" s="44">
+      <c r="D2" s="45">
         <v>1567999.5</v>
       </c>
     </row>
@@ -10107,119 +10110,119 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="52" t="s">
         <v>222</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="52" t="s">
         <v>223</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="52" t="s">
         <v>224</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="52" t="s">
         <v>224</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="52" t="s">
         <v>214</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="52" t="s">
         <v>224</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="H1" s="52" t="s">
         <v>225</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="I1" s="52" t="s">
         <v>215</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="52" t="s">
         <v>215</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="K1" s="52" t="s">
         <v>217</v>
       </c>
-      <c r="L1" s="51" t="s">
+      <c r="L1" s="52" t="s">
         <v>226</v>
       </c>
-      <c r="M1" s="51" t="s">
+      <c r="M1" s="52" t="s">
         <v>226</v>
       </c>
-      <c r="N1" s="51" t="s">
+      <c r="N1" s="52" t="s">
         <v>227</v>
       </c>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="52"/>
+      <c r="R1" s="52"/>
+      <c r="S1" s="52"/>
+      <c r="T1" s="52"/>
+      <c r="U1" s="52"/>
+      <c r="V1" s="52"/>
+      <c r="W1" s="52"/>
+      <c r="X1" s="52"/>
+      <c r="Y1" s="52"/>
+      <c r="Z1" s="52"/>
     </row>
     <row r="2" ht="15.0" customHeight="1">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="52" t="s">
         <v>228</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="53" t="s">
         <v>229</v>
       </c>
-      <c r="F2" s="52" t="s">
+      <c r="F2" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="G2" s="53" t="s">
         <v>230</v>
       </c>
-      <c r="H2" s="52" t="s">
+      <c r="H2" s="53" t="s">
         <v>231</v>
       </c>
-      <c r="I2" s="52" t="s">
+      <c r="I2" s="53" t="s">
         <v>170</v>
       </c>
-      <c r="J2" s="52" t="s">
+      <c r="J2" s="53" t="s">
         <v>232</v>
       </c>
-      <c r="K2" s="52" t="s">
+      <c r="K2" s="53" t="s">
         <v>194</v>
       </c>
-      <c r="L2" s="52" t="s">
+      <c r="L2" s="53" t="s">
         <v>211</v>
       </c>
-      <c r="M2" s="52" t="s">
+      <c r="M2" s="53" t="s">
         <v>212</v>
       </c>
-      <c r="N2" s="52" t="s">
+      <c r="N2" s="53" t="s">
         <v>212</v>
       </c>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
-      <c r="V2" s="51"/>
-      <c r="W2" s="51"/>
-      <c r="X2" s="51"/>
-      <c r="Y2" s="51"/>
-      <c r="Z2" s="51"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="52"/>
+      <c r="R2" s="52"/>
+      <c r="S2" s="52"/>
+      <c r="T2" s="52"/>
+      <c r="U2" s="52"/>
+      <c r="V2" s="52"/>
+      <c r="W2" s="52"/>
+      <c r="X2" s="52"/>
+      <c r="Y2" s="52"/>
+      <c r="Z2" s="52"/>
     </row>
     <row r="3" ht="15.0" customHeight="1">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>233</v>
       </c>
       <c r="B3" s="18" t="s">
@@ -10319,7 +10322,7 @@
       <c r="F5" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="G5" s="53" t="s">
+      <c r="G5" s="54" t="s">
         <v>251</v>
       </c>
       <c r="L5" s="18" t="s">
@@ -10361,7 +10364,7 @@
       <c r="D8" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="E8" s="54" t="s">
+      <c r="E8" s="55" t="s">
         <v>259</v>
       </c>
     </row>
@@ -11650,102 +11653,102 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="2" ht="15.0" customHeight="1">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="56" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="56" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="4" ht="15.0" customHeight="1">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="56" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" ht="15.0" customHeight="1">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="56" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="1">
-      <c r="A7" s="51"/>
-      <c r="B7" s="51" t="s">
+      <c r="A7" s="52"/>
+      <c r="B7" s="52" t="s">
         <v>325</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51" t="s">
+      <c r="C7" s="52"/>
+      <c r="D7" s="52" t="s">
         <v>326</v>
       </c>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51" t="s">
+      <c r="E7" s="52"/>
+      <c r="F7" s="52" t="s">
         <v>327</v>
       </c>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51"/>
-      <c r="M7" s="51"/>
-      <c r="N7" s="51"/>
-      <c r="O7" s="51"/>
-      <c r="P7" s="51"/>
-      <c r="Q7" s="51"/>
-      <c r="R7" s="51"/>
-      <c r="S7" s="51"/>
-      <c r="T7" s="51"/>
-      <c r="U7" s="51"/>
-      <c r="V7" s="51"/>
-      <c r="W7" s="51"/>
-      <c r="X7" s="51"/>
-      <c r="Y7" s="51"/>
-      <c r="Z7" s="51"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="52"/>
+      <c r="N7" s="52"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="52"/>
+      <c r="Q7" s="52"/>
+      <c r="R7" s="52"/>
+      <c r="S7" s="52"/>
+      <c r="T7" s="52"/>
+      <c r="U7" s="52"/>
+      <c r="V7" s="52"/>
+      <c r="W7" s="52"/>
+      <c r="X7" s="52"/>
+      <c r="Y7" s="52"/>
+      <c r="Z7" s="52"/>
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="18" t="s">
         <v>328</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="57"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="58"/>
     </row>
     <row r="9" ht="15.0" customHeight="1">
       <c r="A9" s="18" t="s">
         <v>329</v>
       </c>
-      <c r="B9" s="56"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="57"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="58"/>
     </row>
     <row r="10" ht="15.0" customHeight="1">
       <c r="A10" s="18" t="s">
         <v>330</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="56">
+      <c r="B10" s="58"/>
+      <c r="C10" s="57">
         <f>B8+B9</f>
         <v>0</v>
       </c>
-      <c r="D10" s="57"/>
-      <c r="E10" s="56">
+      <c r="D10" s="58"/>
+      <c r="E10" s="57">
         <f>D8+D9</f>
         <v>0</v>
       </c>
-      <c r="F10" s="57"/>
-      <c r="G10" s="56">
+      <c r="F10" s="58"/>
+      <c r="G10" s="57">
         <f>F8+F9</f>
         <v>0</v>
       </c>
@@ -11754,40 +11757,40 @@
       <c r="A11" s="18" t="s">
         <v>331</v>
       </c>
-      <c r="B11" s="56"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="57"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="58"/>
     </row>
     <row r="12" ht="15.0" customHeight="1">
       <c r="A12" s="18" t="s">
         <v>332</v>
       </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="57"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="58"/>
     </row>
     <row r="13" ht="15.0" customHeight="1">
       <c r="A13" s="18" t="s">
         <v>333</v>
       </c>
-      <c r="B13" s="57"/>
-      <c r="C13" s="56">
+      <c r="B13" s="58"/>
+      <c r="C13" s="57">
         <f>B11+B12</f>
         <v>0</v>
       </c>
-      <c r="D13" s="57"/>
-      <c r="E13" s="56">
+      <c r="D13" s="58"/>
+      <c r="E13" s="57">
         <f>D11+D12</f>
         <v>0</v>
       </c>
-      <c r="F13" s="57"/>
-      <c r="G13" s="56">
+      <c r="F13" s="58"/>
+      <c r="G13" s="57">
         <f>F11+F12</f>
         <v>0</v>
       </c>
@@ -11796,40 +11799,40 @@
       <c r="A14" s="18" t="s">
         <v>334</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="57"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="58"/>
     </row>
     <row r="15" ht="15.0" customHeight="1">
       <c r="A15" s="18" t="s">
         <v>335</v>
       </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="57"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="58"/>
     </row>
     <row r="16" ht="15.0" customHeight="1">
       <c r="A16" s="18" t="s">
         <v>336</v>
       </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="56">
+      <c r="B16" s="58"/>
+      <c r="C16" s="57">
         <f>B14+B15</f>
         <v>0</v>
       </c>
-      <c r="D16" s="57"/>
-      <c r="E16" s="56">
+      <c r="D16" s="58"/>
+      <c r="E16" s="57">
         <f>D14+D15</f>
         <v>0</v>
       </c>
-      <c r="F16" s="57"/>
-      <c r="G16" s="56">
+      <c r="F16" s="58"/>
+      <c r="G16" s="57">
         <f>F14+F15</f>
         <v>0</v>
       </c>
@@ -11838,40 +11841,40 @@
       <c r="A17" s="18" t="s">
         <v>337</v>
       </c>
-      <c r="B17" s="56"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="57"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="58"/>
     </row>
     <row r="18" ht="15.0" customHeight="1">
       <c r="A18" s="18" t="s">
         <v>338</v>
       </c>
-      <c r="B18" s="56"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="57"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="58"/>
     </row>
     <row r="19" ht="15.0" customHeight="1">
       <c r="A19" s="18" t="s">
         <v>339</v>
       </c>
-      <c r="B19" s="57"/>
-      <c r="C19" s="56">
+      <c r="B19" s="58"/>
+      <c r="C19" s="57">
         <f>B17+B18</f>
         <v>0</v>
       </c>
-      <c r="D19" s="57"/>
-      <c r="E19" s="56">
+      <c r="D19" s="58"/>
+      <c r="E19" s="57">
         <f>D17+D18</f>
         <v>0</v>
       </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="56">
+      <c r="F19" s="58"/>
+      <c r="G19" s="57">
         <f>F17+F18</f>
         <v>0</v>
       </c>
@@ -11880,40 +11883,40 @@
       <c r="A20" s="18" t="s">
         <v>340</v>
       </c>
-      <c r="B20" s="56"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="57"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="58"/>
     </row>
     <row r="21" ht="15.0" customHeight="1">
       <c r="A21" s="18" t="s">
         <v>341</v>
       </c>
-      <c r="B21" s="56"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="57"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="57"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="58"/>
     </row>
     <row r="22" ht="15.0" customHeight="1">
       <c r="A22" s="18" t="s">
         <v>342</v>
       </c>
-      <c r="B22" s="57"/>
-      <c r="C22" s="56">
+      <c r="B22" s="58"/>
+      <c r="C22" s="57">
         <f>B20+B21</f>
         <v>0</v>
       </c>
-      <c r="D22" s="57"/>
-      <c r="E22" s="56">
+      <c r="D22" s="58"/>
+      <c r="E22" s="57">
         <f>D20+D21</f>
         <v>0</v>
       </c>
-      <c r="F22" s="57"/>
-      <c r="G22" s="56">
+      <c r="F22" s="58"/>
+      <c r="G22" s="57">
         <f>F20+F21</f>
         <v>0</v>
       </c>
@@ -11922,51 +11925,51 @@
       <c r="A23" s="18" t="s">
         <v>343</v>
       </c>
-      <c r="B23" s="57"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="56"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="57"/>
     </row>
     <row r="24" ht="15.0" customHeight="1">
-      <c r="A24" s="51" t="s">
+      <c r="A24" s="52" t="s">
         <v>344</v>
       </c>
-      <c r="B24" s="58"/>
-      <c r="C24" s="58">
+      <c r="B24" s="59"/>
+      <c r="C24" s="59">
         <f>C10+C13+C16+C19+C22</f>
         <v>0</v>
       </c>
-      <c r="D24" s="58"/>
-      <c r="E24" s="58">
+      <c r="D24" s="59"/>
+      <c r="E24" s="59">
         <f>E10+E13+E16+E19+E22</f>
         <v>0</v>
       </c>
-      <c r="F24" s="58"/>
-      <c r="G24" s="58">
+      <c r="F24" s="59"/>
+      <c r="G24" s="59">
         <f>G10+G13+G16+G19+G22</f>
         <v>0</v>
       </c>
-      <c r="H24" s="51"/>
-      <c r="I24" s="51"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="51"/>
-      <c r="L24" s="51"/>
-      <c r="M24" s="51"/>
-      <c r="N24" s="51"/>
-      <c r="O24" s="51"/>
-      <c r="P24" s="51"/>
-      <c r="Q24" s="51"/>
-      <c r="R24" s="51"/>
-      <c r="S24" s="51"/>
-      <c r="T24" s="51"/>
-      <c r="U24" s="51"/>
-      <c r="V24" s="51"/>
-      <c r="W24" s="51"/>
-      <c r="X24" s="51"/>
-      <c r="Y24" s="51"/>
-      <c r="Z24" s="51"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="52"/>
+      <c r="N24" s="52"/>
+      <c r="O24" s="52"/>
+      <c r="P24" s="52"/>
+      <c r="Q24" s="52"/>
+      <c r="R24" s="52"/>
+      <c r="S24" s="52"/>
+      <c r="T24" s="52"/>
+      <c r="U24" s="52"/>
+      <c r="V24" s="52"/>
+      <c r="W24" s="52"/>
+      <c r="X24" s="52"/>
+      <c r="Y24" s="52"/>
+      <c r="Z24" s="52"/>
     </row>
     <row r="25" ht="15.75" customHeight="1"/>
     <row r="26" ht="15.75" customHeight="1"/>
@@ -28022,8 +28025,8 @@
       <c r="C4" s="22" t="s">
         <v>198</v>
       </c>
-      <c r="D4" s="22">
-        <v>50856.3</v>
+      <c r="D4" s="41">
+        <v>2050856.3</v>
       </c>
       <c r="E4" s="24">
         <v>44005.0</v>
@@ -32906,22 +32909,22 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="42">
+      <c r="C2" s="43">
         <v>2.101184477E7</v>
       </c>
-      <c r="D2" s="43">
+      <c r="D2" s="44">
         <v>44008.0</v>
       </c>
       <c r="E2" s="36">
         <v>75.0</v>
       </c>
-      <c r="F2" s="42">
+      <c r="F2" s="43">
         <v>2.101184477E7</v>
       </c>
       <c r="G2" s="8">
@@ -32930,12 +32933,12 @@
       <c r="H2" s="8">
         <v>44012.0</v>
       </c>
-      <c r="I2" s="42">
+      <c r="I2" s="43">
         <v>2.101184477E7</v>
       </c>
       <c r="J2" s="13"/>
       <c r="K2" s="13"/>
-      <c r="L2" s="44">
+      <c r="L2" s="45">
         <v>1.0505922385E7</v>
       </c>
       <c r="M2" s="13"/>
@@ -32948,22 +32951,22 @@
       <c r="R2" s="13"/>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="46">
+      <c r="C3" s="47">
         <v>1.578213759E7</v>
       </c>
-      <c r="D3" s="47">
+      <c r="D3" s="48">
         <v>44008.0</v>
       </c>
       <c r="E3" s="36">
         <v>75.0</v>
       </c>
-      <c r="F3" s="46">
+      <c r="F3" s="47">
         <v>1.578213759E7</v>
       </c>
       <c r="G3" s="8">
@@ -32972,12 +32975,12 @@
       <c r="H3" s="8">
         <v>44012.0</v>
       </c>
-      <c r="I3" s="46">
+      <c r="I3" s="47">
         <v>1.578213759E7</v>
       </c>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
-      <c r="L3" s="44">
+      <c r="L3" s="45">
         <v>1.578213759E7</v>
       </c>
       <c r="M3" s="13"/>
@@ -32988,22 +32991,22 @@
       <c r="R3" s="13"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="48">
+      <c r="C4" s="49">
         <v>1.0964770477E8</v>
       </c>
-      <c r="D4" s="43">
+      <c r="D4" s="44">
         <v>44008.0</v>
       </c>
       <c r="E4" s="36">
         <v>75.0</v>
       </c>
-      <c r="F4" s="42">
+      <c r="F4" s="43">
         <v>9647704.77</v>
       </c>
       <c r="G4" s="8">
@@ -33012,12 +33015,12 @@
       <c r="H4" s="8">
         <v>44012.0</v>
       </c>
-      <c r="I4" s="42">
+      <c r="I4" s="43">
         <v>9647704.77</v>
       </c>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="44">
+      <c r="L4" s="45">
         <v>4823852.385</v>
       </c>
       <c r="M4" s="13"/>
@@ -33026,7 +33029,7 @@
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
       <c r="R4" s="13"/>
-      <c r="T4" s="44">
+      <c r="T4" s="45">
         <v>4823852.385</v>
       </c>
     </row>
@@ -33067,7 +33070,7 @@
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="K10" s="13"/>
-      <c r="M10" s="49"/>
+      <c r="M10" s="50"/>
       <c r="O10" s="13"/>
       <c r="Q10" s="13"/>
       <c r="R10" s="13"/>

</xml_diff>

<commit_message>
add cumulative validations for transfers
</commit_message>
<xml_diff>
--- a/tests/server/fixtures/file-success/EOHHS-075-12312020-simple-v1.xlsx
+++ b/tests/server/fixtures/file-success/EOHHS-075-12312020-simple-v1.xlsx
@@ -30422,8 +30422,8 @@
       <c r="C2" s="22" t="s">
         <v>205</v>
       </c>
-      <c r="D2" s="29">
-        <v>32416.32</v>
+      <c r="D2" s="27">
+        <v>132416.32</v>
       </c>
       <c r="E2" s="24">
         <v>43987.643125</v>

</xml_diff>

<commit_message>
add cumulative expenditure validation for contracts, direct, grants, loans
</commit_message>
<xml_diff>
--- a/tests/server/fixtures/file-success/EOHHS-075-12312020-simple-v1.xlsx
+++ b/tests/server/fixtures/file-success/EOHHS-075-12312020-simple-v1.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="345">
   <si>
     <t>Certification</t>
   </si>
@@ -541,9 +541,6 @@
     <t>60060</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>3674861</t>
   </si>
   <si>
@@ -899,6 +896,9 @@
   </si>
   <si>
     <t>ME</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
   <si>
     <t>MH</t>
@@ -1318,7 +1318,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="58">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1388,13 +1388,7 @@
     <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="6" fillId="0" fontId="4" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="5" fillId="0" fontId="4" numFmtId="14" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="5" fillId="0" fontId="4" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="4" fillId="8" fontId="4" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="1" fillId="8" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -7974,70 +7968,70 @@
   <sheetData>
     <row r="1" ht="37.5" customHeight="1">
       <c r="A1" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>135</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B2" s="18"/>
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B3" s="18">
         <v>75.0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="D3" s="51">
+        <v>215</v>
+      </c>
+      <c r="D3" s="49">
         <v>2163121.97</v>
       </c>
-      <c r="E3" s="51">
+      <c r="E3" s="49">
         <v>840542.45</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B4" s="18">
         <v>75.0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="D4" s="51">
+        <v>180</v>
+      </c>
+      <c r="D4" s="49">
         <v>5957909.0</v>
       </c>
-      <c r="E4" s="51">
+      <c r="E4" s="49">
         <v>5957909.0</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B5" s="18"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B6" s="18"/>
     </row>
@@ -9064,26 +9058,26 @@
         <v>6</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>135</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="36">
+      <c r="A2" s="34">
         <v>75.0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C2" s="45">
+        <v>180</v>
+      </c>
+      <c r="C2" s="43">
         <v>1567999.5</v>
       </c>
-      <c r="D2" s="45">
+      <c r="D2" s="43">
         <v>1567999.5</v>
       </c>
     </row>
@@ -10110,262 +10104,262 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="50" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="50" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="C1" s="50" t="s">
         <v>222</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="D1" s="50" t="s">
         <v>223</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="E1" s="50" t="s">
+        <v>223</v>
+      </c>
+      <c r="F1" s="50" t="s">
+        <v>213</v>
+      </c>
+      <c r="G1" s="50" t="s">
+        <v>223</v>
+      </c>
+      <c r="H1" s="50" t="s">
         <v>224</v>
       </c>
-      <c r="E1" s="52" t="s">
-        <v>224</v>
-      </c>
-      <c r="F1" s="52" t="s">
+      <c r="I1" s="50" t="s">
         <v>214</v>
       </c>
-      <c r="G1" s="52" t="s">
-        <v>224</v>
-      </c>
-      <c r="H1" s="52" t="s">
+      <c r="J1" s="50" t="s">
+        <v>214</v>
+      </c>
+      <c r="K1" s="50" t="s">
+        <v>216</v>
+      </c>
+      <c r="L1" s="50" t="s">
         <v>225</v>
       </c>
-      <c r="I1" s="52" t="s">
-        <v>215</v>
-      </c>
-      <c r="J1" s="52" t="s">
-        <v>215</v>
-      </c>
-      <c r="K1" s="52" t="s">
-        <v>217</v>
-      </c>
-      <c r="L1" s="52" t="s">
+      <c r="M1" s="50" t="s">
+        <v>225</v>
+      </c>
+      <c r="N1" s="50" t="s">
         <v>226</v>
       </c>
-      <c r="M1" s="52" t="s">
-        <v>226</v>
-      </c>
-      <c r="N1" s="52" t="s">
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="50"/>
+    </row>
+    <row r="2" ht="15.0" customHeight="1">
+      <c r="A2" s="50" t="s">
         <v>227</v>
       </c>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
-    </row>
-    <row r="2" ht="15.0" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="B2" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="51" t="s">
         <v>228</v>
       </c>
-      <c r="B2" s="53" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="53" t="s">
+      <c r="F2" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="51" t="s">
         <v>229</v>
       </c>
-      <c r="F2" s="53" t="s">
-        <v>120</v>
-      </c>
-      <c r="G2" s="53" t="s">
+      <c r="H2" s="51" t="s">
         <v>230</v>
       </c>
-      <c r="H2" s="53" t="s">
+      <c r="I2" s="51" t="s">
+        <v>169</v>
+      </c>
+      <c r="J2" s="51" t="s">
         <v>231</v>
       </c>
-      <c r="I2" s="53" t="s">
-        <v>170</v>
-      </c>
-      <c r="J2" s="53" t="s">
+      <c r="K2" s="51" t="s">
+        <v>193</v>
+      </c>
+      <c r="L2" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="M2" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="N2" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="50"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="50"/>
+      <c r="X2" s="50"/>
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="50"/>
+    </row>
+    <row r="3" ht="15.0" customHeight="1">
+      <c r="A3" s="50" t="s">
         <v>232</v>
-      </c>
-      <c r="K2" s="53" t="s">
-        <v>194</v>
-      </c>
-      <c r="L2" s="53" t="s">
-        <v>211</v>
-      </c>
-      <c r="M2" s="53" t="s">
-        <v>212</v>
-      </c>
-      <c r="N2" s="53" t="s">
-        <v>212</v>
-      </c>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
-      <c r="R2" s="52"/>
-      <c r="S2" s="52"/>
-      <c r="T2" s="52"/>
-      <c r="U2" s="52"/>
-      <c r="V2" s="52"/>
-      <c r="W2" s="52"/>
-      <c r="X2" s="52"/>
-      <c r="Y2" s="52"/>
-      <c r="Z2" s="52"/>
-    </row>
-    <row r="3" ht="15.0" customHeight="1">
-      <c r="A3" s="52" t="s">
-        <v>233</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" s="18" t="s">
         <v>234</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="E3" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="F3" s="18" t="s">
         <v>236</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>237</v>
       </c>
       <c r="G3" s="18">
         <v>1.0</v>
       </c>
       <c r="H3" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="I3" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="I3" s="18" t="s">
-        <v>239</v>
-      </c>
       <c r="J3" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K3" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L3" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N3" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" ht="15.0" customHeight="1">
       <c r="B4" s="18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>55</v>
       </c>
       <c r="D4" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="F4" s="18" t="s">
         <v>242</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>243</v>
       </c>
       <c r="G4" s="18">
         <v>2.0</v>
       </c>
       <c r="H4" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="J4" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="I4" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="J4" s="18" t="s">
+      <c r="K4" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="K4" s="18" t="s">
-        <v>246</v>
-      </c>
       <c r="L4" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="M4" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N4" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" ht="15.0" customHeight="1">
       <c r="B5" s="18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>62</v>
       </c>
       <c r="D5" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="E5" s="18" t="s">
         <v>248</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="F5" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="G5" s="52" t="s">
         <v>250</v>
       </c>
-      <c r="G5" s="54" t="s">
-        <v>251</v>
-      </c>
       <c r="L5" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" ht="15.0" customHeight="1">
       <c r="B6" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>68</v>
       </c>
       <c r="D6" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="F6" s="18" t="s">
-        <v>254</v>
-      </c>
       <c r="L6" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="C7" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="L7" s="18" t="s">
         <v>256</v>
-      </c>
-      <c r="L7" s="18" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="C8" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="E8" s="55" t="s">
-        <v>259</v>
+      <c r="E8" s="53" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="9" ht="15.0" customHeight="1">
@@ -10373,7 +10367,7 @@
         <v>80</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10" ht="15.0" customHeight="1">
@@ -10381,7 +10375,7 @@
         <v>88</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11" ht="15.0" customHeight="1">
@@ -10389,15 +10383,15 @@
         <v>93</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="12" ht="15.0" customHeight="1">
       <c r="C12" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="D12" s="18" t="s">
         <v>263</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="13" ht="15.0" customHeight="1">
@@ -10405,7 +10399,7 @@
         <v>104</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" ht="15.0" customHeight="1">
@@ -10413,7 +10407,7 @@
         <v>110</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" ht="15.0" customHeight="1">
@@ -10421,36 +10415,36 @@
         <v>116</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" ht="15.0" customHeight="1">
       <c r="C16" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="D16" s="18" t="s">
         <v>268</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="17" ht="15.0" customHeight="1">
       <c r="C17" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="D17" s="18" t="s">
         <v>270</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="18" ht="15.0" customHeight="1">
       <c r="C18" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="D18" s="18" t="s">
         <v>272</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="19" ht="15.0" customHeight="1">
       <c r="C19" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>165</v>
@@ -10458,55 +10452,55 @@
     </row>
     <row r="20" ht="15.0" customHeight="1">
       <c r="C20" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="D20" s="18" t="s">
         <v>275</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="21" ht="15.0" customHeight="1">
       <c r="C21" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="D21" s="18" t="s">
         <v>277</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="22" ht="15.0" customHeight="1">
       <c r="C22" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="D22" s="18" t="s">
         <v>279</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="23" ht="15.0" customHeight="1">
       <c r="C23" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="D23" s="18" t="s">
         <v>281</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="24" ht="15.0" customHeight="1">
       <c r="C24" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="D24" s="18" t="s">
         <v>283</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="25" ht="15.0" customHeight="1">
       <c r="C25" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="D25" s="18" t="s">
         <v>285</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="26" ht="15.0" customHeight="1">
       <c r="C26" s="18" t="s">
-        <v>167</v>
+        <v>286</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>287</v>
@@ -11653,102 +11647,102 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="50" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="2" ht="15.0" customHeight="1">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="54" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="1">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="54" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="4" ht="15.0" customHeight="1">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="54" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" ht="15.0" customHeight="1">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="54" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="1">
-      <c r="A7" s="52"/>
-      <c r="B7" s="52" t="s">
+      <c r="A7" s="50"/>
+      <c r="B7" s="50" t="s">
         <v>325</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52" t="s">
+      <c r="C7" s="50"/>
+      <c r="D7" s="50" t="s">
         <v>326</v>
       </c>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52" t="s">
+      <c r="E7" s="50"/>
+      <c r="F7" s="50" t="s">
         <v>327</v>
       </c>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="52"/>
-      <c r="N7" s="52"/>
-      <c r="O7" s="52"/>
-      <c r="P7" s="52"/>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="52"/>
-      <c r="S7" s="52"/>
-      <c r="T7" s="52"/>
-      <c r="U7" s="52"/>
-      <c r="V7" s="52"/>
-      <c r="W7" s="52"/>
-      <c r="X7" s="52"/>
-      <c r="Y7" s="52"/>
-      <c r="Z7" s="52"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="50"/>
+      <c r="R7" s="50"/>
+      <c r="S7" s="50"/>
+      <c r="T7" s="50"/>
+      <c r="U7" s="50"/>
+      <c r="V7" s="50"/>
+      <c r="W7" s="50"/>
+      <c r="X7" s="50"/>
+      <c r="Y7" s="50"/>
+      <c r="Z7" s="50"/>
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="18" t="s">
         <v>328</v>
       </c>
-      <c r="B8" s="57"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="58"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="56"/>
     </row>
     <row r="9" ht="15.0" customHeight="1">
       <c r="A9" s="18" t="s">
         <v>329</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="58"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="56"/>
     </row>
     <row r="10" ht="15.0" customHeight="1">
       <c r="A10" s="18" t="s">
         <v>330</v>
       </c>
-      <c r="B10" s="58"/>
-      <c r="C10" s="57">
+      <c r="B10" s="56"/>
+      <c r="C10" s="55">
         <f>B8+B9</f>
         <v>0</v>
       </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="57">
+      <c r="D10" s="56"/>
+      <c r="E10" s="55">
         <f>D8+D9</f>
         <v>0</v>
       </c>
-      <c r="F10" s="58"/>
-      <c r="G10" s="57">
+      <c r="F10" s="56"/>
+      <c r="G10" s="55">
         <f>F8+F9</f>
         <v>0</v>
       </c>
@@ -11757,40 +11751,40 @@
       <c r="A11" s="18" t="s">
         <v>331</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="58"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="56"/>
     </row>
     <row r="12" ht="15.0" customHeight="1">
       <c r="A12" s="18" t="s">
         <v>332</v>
       </c>
-      <c r="B12" s="57"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="58"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="56"/>
     </row>
     <row r="13" ht="15.0" customHeight="1">
       <c r="A13" s="18" t="s">
         <v>333</v>
       </c>
-      <c r="B13" s="58"/>
-      <c r="C13" s="57">
+      <c r="B13" s="56"/>
+      <c r="C13" s="55">
         <f>B11+B12</f>
         <v>0</v>
       </c>
-      <c r="D13" s="58"/>
-      <c r="E13" s="57">
+      <c r="D13" s="56"/>
+      <c r="E13" s="55">
         <f>D11+D12</f>
         <v>0</v>
       </c>
-      <c r="F13" s="58"/>
-      <c r="G13" s="57">
+      <c r="F13" s="56"/>
+      <c r="G13" s="55">
         <f>F11+F12</f>
         <v>0</v>
       </c>
@@ -11799,40 +11793,40 @@
       <c r="A14" s="18" t="s">
         <v>334</v>
       </c>
-      <c r="B14" s="57"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="58"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="56"/>
     </row>
     <row r="15" ht="15.0" customHeight="1">
       <c r="A15" s="18" t="s">
         <v>335</v>
       </c>
-      <c r="B15" s="57"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="58"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="56"/>
     </row>
     <row r="16" ht="15.0" customHeight="1">
       <c r="A16" s="18" t="s">
         <v>336</v>
       </c>
-      <c r="B16" s="58"/>
-      <c r="C16" s="57">
+      <c r="B16" s="56"/>
+      <c r="C16" s="55">
         <f>B14+B15</f>
         <v>0</v>
       </c>
-      <c r="D16" s="58"/>
-      <c r="E16" s="57">
+      <c r="D16" s="56"/>
+      <c r="E16" s="55">
         <f>D14+D15</f>
         <v>0</v>
       </c>
-      <c r="F16" s="58"/>
-      <c r="G16" s="57">
+      <c r="F16" s="56"/>
+      <c r="G16" s="55">
         <f>F14+F15</f>
         <v>0</v>
       </c>
@@ -11841,40 +11835,40 @@
       <c r="A17" s="18" t="s">
         <v>337</v>
       </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="58"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="56"/>
     </row>
     <row r="18" ht="15.0" customHeight="1">
       <c r="A18" s="18" t="s">
         <v>338</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="58"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="56"/>
     </row>
     <row r="19" ht="15.0" customHeight="1">
       <c r="A19" s="18" t="s">
         <v>339</v>
       </c>
-      <c r="B19" s="58"/>
-      <c r="C19" s="57">
+      <c r="B19" s="56"/>
+      <c r="C19" s="55">
         <f>B17+B18</f>
         <v>0</v>
       </c>
-      <c r="D19" s="58"/>
-      <c r="E19" s="57">
+      <c r="D19" s="56"/>
+      <c r="E19" s="55">
         <f>D17+D18</f>
         <v>0</v>
       </c>
-      <c r="F19" s="58"/>
-      <c r="G19" s="57">
+      <c r="F19" s="56"/>
+      <c r="G19" s="55">
         <f>F17+F18</f>
         <v>0</v>
       </c>
@@ -11883,40 +11877,40 @@
       <c r="A20" s="18" t="s">
         <v>340</v>
       </c>
-      <c r="B20" s="57"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="58"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="56"/>
     </row>
     <row r="21" ht="15.0" customHeight="1">
       <c r="A21" s="18" t="s">
         <v>341</v>
       </c>
-      <c r="B21" s="57"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="58"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="56"/>
     </row>
     <row r="22" ht="15.0" customHeight="1">
       <c r="A22" s="18" t="s">
         <v>342</v>
       </c>
-      <c r="B22" s="58"/>
-      <c r="C22" s="57">
+      <c r="B22" s="56"/>
+      <c r="C22" s="55">
         <f>B20+B21</f>
         <v>0</v>
       </c>
-      <c r="D22" s="58"/>
-      <c r="E22" s="57">
+      <c r="D22" s="56"/>
+      <c r="E22" s="55">
         <f>D20+D21</f>
         <v>0</v>
       </c>
-      <c r="F22" s="58"/>
-      <c r="G22" s="57">
+      <c r="F22" s="56"/>
+      <c r="G22" s="55">
         <f>F20+F21</f>
         <v>0</v>
       </c>
@@ -11925,51 +11919,51 @@
       <c r="A23" s="18" t="s">
         <v>343</v>
       </c>
-      <c r="B23" s="58"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="58"/>
-      <c r="G23" s="57"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="55"/>
     </row>
     <row r="24" ht="15.0" customHeight="1">
-      <c r="A24" s="52" t="s">
+      <c r="A24" s="50" t="s">
         <v>344</v>
       </c>
-      <c r="B24" s="59"/>
-      <c r="C24" s="59">
+      <c r="B24" s="57"/>
+      <c r="C24" s="57">
         <f>C10+C13+C16+C19+C22</f>
         <v>0</v>
       </c>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59">
+      <c r="D24" s="57"/>
+      <c r="E24" s="57">
         <f>E10+E13+E16+E19+E22</f>
         <v>0</v>
       </c>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59">
+      <c r="F24" s="57"/>
+      <c r="G24" s="57">
         <f>G10+G13+G16+G19+G22</f>
         <v>0</v>
       </c>
-      <c r="H24" s="52"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="52"/>
-      <c r="L24" s="52"/>
-      <c r="M24" s="52"/>
-      <c r="N24" s="52"/>
-      <c r="O24" s="52"/>
-      <c r="P24" s="52"/>
-      <c r="Q24" s="52"/>
-      <c r="R24" s="52"/>
-      <c r="S24" s="52"/>
-      <c r="T24" s="52"/>
-      <c r="U24" s="52"/>
-      <c r="V24" s="52"/>
-      <c r="W24" s="52"/>
-      <c r="X24" s="52"/>
-      <c r="Y24" s="52"/>
-      <c r="Z24" s="52"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="50"/>
+      <c r="L24" s="50"/>
+      <c r="M24" s="50"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="50"/>
+      <c r="P24" s="50"/>
+      <c r="Q24" s="50"/>
+      <c r="R24" s="50"/>
+      <c r="S24" s="50"/>
+      <c r="T24" s="50"/>
+      <c r="U24" s="50"/>
+      <c r="V24" s="50"/>
+      <c r="W24" s="50"/>
+      <c r="X24" s="50"/>
+      <c r="Y24" s="50"/>
+      <c r="Z24" s="50"/>
     </row>
     <row r="25" ht="15.75" customHeight="1"/>
     <row r="26" ht="15.75" customHeight="1"/>
@@ -20366,11 +20360,9 @@
         <v>44012.0</v>
       </c>
       <c r="V2" s="27">
-        <v>100172.0</v>
-      </c>
-      <c r="W2" s="28">
-        <v>100000.0</v>
-      </c>
+        <v>172.0</v>
+      </c>
+      <c r="W2" s="28"/>
       <c r="X2" s="13"/>
       <c r="Y2" s="13"/>
       <c r="Z2" s="13"/>
@@ -20440,27 +20432,20 @@
         <v>44012.0</v>
       </c>
       <c r="V3" s="33">
-        <v>119199.25</v>
-      </c>
-      <c r="W3" s="28">
-        <v>100000.0</v>
-      </c>
+        <v>9199.25</v>
+      </c>
+      <c r="W3" s="28"/>
       <c r="X3" s="13"/>
       <c r="Y3" s="13"/>
       <c r="Z3" s="13"/>
       <c r="AA3" s="13"/>
       <c r="AB3" s="13"/>
       <c r="AC3" s="13"/>
-      <c r="AD3" s="34">
+      <c r="AD3" s="33">
         <v>9199.25</v>
       </c>
       <c r="AE3" s="13"/>
-      <c r="AN3" s="35" t="s">
-        <v>167</v>
-      </c>
-      <c r="AO3" s="36">
-        <v>10000.0</v>
-      </c>
+      <c r="AO3" s="34"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" s="22" t="s">
@@ -20470,12 +20455,12 @@
         <v>100</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="E4" s="37">
+      <c r="E4" s="35">
         <v>27620.0</v>
       </c>
       <c r="F4" s="24">
@@ -20510,7 +20495,7 @@
       <c r="R4" s="13">
         <v>75.0</v>
       </c>
-      <c r="S4" s="37">
+      <c r="S4" s="35">
         <v>27620.0</v>
       </c>
       <c r="T4" s="24">
@@ -20519,12 +20504,10 @@
       <c r="U4" s="26">
         <v>44012.0</v>
       </c>
-      <c r="V4" s="27">
-        <v>113810.0</v>
-      </c>
-      <c r="W4" s="28">
-        <v>100000.0</v>
-      </c>
+      <c r="V4" s="29">
+        <v>13810.0</v>
+      </c>
+      <c r="W4" s="28"/>
       <c r="X4" s="13"/>
       <c r="Y4" s="13"/>
       <c r="Z4" s="13"/>
@@ -23042,16 +23025,16 @@
         <v>118</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="10" t="s">
         <v>171</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>172</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>123</v>
@@ -23060,13 +23043,13 @@
         <v>124</v>
       </c>
       <c r="I1" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="J1" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>174</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>175</v>
       </c>
       <c r="L1" s="10" t="s">
         <v>128</v>
@@ -23078,19 +23061,19 @@
         <v>130</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P1" s="10" t="s">
         <v>132</v>
       </c>
       <c r="Q1" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="R1" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>178</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>179</v>
       </c>
       <c r="T1" s="10" t="s">
         <v>134</v>
@@ -23175,11 +23158,11 @@
       <c r="B2" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="36">
+      <c r="C2" s="34">
         <v>1234.0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E2" s="23">
         <v>1.29276E7</v>
@@ -23210,20 +23193,20 @@
       <c r="O2" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="R2" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="T2" s="36">
+      <c r="R2" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="T2" s="34">
         <v>75.0</v>
       </c>
-      <c r="U2" s="37">
+      <c r="U2" s="35">
         <v>2927600.0</v>
       </c>
       <c r="V2" s="24">
         <v>43969.64884259259</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="X2" s="29">
         <v>585520.0</v>
@@ -27788,22 +27771,22 @@
         <v>117</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>187</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>188</v>
       </c>
       <c r="H1" s="10" t="s">
         <v>126</v>
@@ -27812,22 +27795,22 @@
         <v>127</v>
       </c>
       <c r="J1" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="K1" s="10" t="s">
         <v>189</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>190</v>
       </c>
       <c r="L1" s="10" t="s">
         <v>130</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N1" s="10" t="s">
         <v>132</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="P1" s="10" t="s">
         <v>135</v>
@@ -27836,13 +27819,13 @@
         <v>134</v>
       </c>
       <c r="R1" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="S1" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>193</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>194</v>
       </c>
       <c r="U1" s="21" t="s">
         <v>139</v>
@@ -27906,14 +27889,14 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="37" t="s">
         <v>69</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D2" s="22">
         <v>50311.8</v>
@@ -27945,31 +27928,31 @@
       <c r="M2" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="38" t="s">
-        <v>196</v>
+      <c r="O2" s="36" t="s">
+        <v>195</v>
       </c>
       <c r="P2" s="22">
         <v>50311.8</v>
       </c>
-      <c r="Q2" s="36">
+      <c r="Q2" s="34">
         <v>75.0</v>
       </c>
-      <c r="T2" s="36" t="s">
-        <v>181</v>
+      <c r="T2" s="34" t="s">
+        <v>180</v>
       </c>
       <c r="AC2" s="22">
         <v>50311.8</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="38" t="s">
         <v>89</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>90</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D3" s="30">
         <v>50529.6</v>
@@ -27999,33 +27982,33 @@
       <c r="M3" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="O3" s="38" t="s">
-        <v>196</v>
+      <c r="O3" s="36" t="s">
+        <v>195</v>
       </c>
       <c r="P3" s="30">
         <v>50529.6</v>
       </c>
-      <c r="Q3" s="36">
+      <c r="Q3" s="34">
         <v>75.0</v>
       </c>
-      <c r="T3" s="36" t="s">
-        <v>181</v>
+      <c r="T3" s="34" t="s">
+        <v>180</v>
       </c>
       <c r="AC3" s="30">
         <v>50529.6</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="37" t="s">
         <v>63</v>
       </c>
       <c r="B4" s="22" t="s">
         <v>64</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>198</v>
-      </c>
-      <c r="D4" s="41">
+        <v>197</v>
+      </c>
+      <c r="D4" s="39">
         <v>2050856.3</v>
       </c>
       <c r="E4" s="24">
@@ -28055,24 +28038,24 @@
       <c r="M4" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="O4" s="38" t="s">
-        <v>196</v>
+      <c r="O4" s="36" t="s">
+        <v>195</v>
       </c>
       <c r="P4" s="22">
         <v>50856.3</v>
       </c>
-      <c r="Q4" s="36">
+      <c r="Q4" s="34">
         <v>75.0</v>
       </c>
-      <c r="T4" s="36" t="s">
-        <v>181</v>
+      <c r="T4" s="34" t="s">
+        <v>180</v>
       </c>
       <c r="AC4" s="22">
         <v>50856.3</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="40"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="30"/>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -28085,12 +28068,12 @@
       <c r="K5" s="30"/>
       <c r="L5" s="30"/>
       <c r="M5" s="30"/>
-      <c r="O5" s="38"/>
+      <c r="O5" s="36"/>
       <c r="P5" s="30"/>
       <c r="AC5" s="30"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="39"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
@@ -28103,12 +28086,12 @@
       <c r="K6" s="22"/>
       <c r="L6" s="22"/>
       <c r="M6" s="22"/>
-      <c r="O6" s="38"/>
+      <c r="O6" s="36"/>
       <c r="P6" s="22"/>
       <c r="AC6" s="22"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="40"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="30"/>
       <c r="C7" s="30"/>
       <c r="D7" s="30"/>
@@ -28121,12 +28104,12 @@
       <c r="K7" s="30"/>
       <c r="L7" s="30"/>
       <c r="M7" s="30"/>
-      <c r="O7" s="38"/>
+      <c r="O7" s="36"/>
       <c r="P7" s="30"/>
       <c r="AC7" s="30"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="39"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -28139,12 +28122,12 @@
       <c r="K8" s="22"/>
       <c r="L8" s="22"/>
       <c r="M8" s="22"/>
-      <c r="O8" s="38"/>
+      <c r="O8" s="36"/>
       <c r="P8" s="22"/>
       <c r="AC8" s="22"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="40"/>
+      <c r="A9" s="38"/>
       <c r="B9" s="30"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
@@ -28157,12 +28140,12 @@
       <c r="K9" s="30"/>
       <c r="L9" s="30"/>
       <c r="M9" s="30"/>
-      <c r="O9" s="38"/>
+      <c r="O9" s="36"/>
       <c r="P9" s="30"/>
       <c r="AC9" s="30"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="39"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
@@ -28175,12 +28158,12 @@
       <c r="K10" s="22"/>
       <c r="L10" s="22"/>
       <c r="M10" s="22"/>
-      <c r="O10" s="38"/>
+      <c r="O10" s="36"/>
       <c r="P10" s="22"/>
       <c r="AC10" s="22"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="40"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="30"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
@@ -28193,12 +28176,12 @@
       <c r="K11" s="30"/>
       <c r="L11" s="30"/>
       <c r="M11" s="30"/>
-      <c r="O11" s="38"/>
+      <c r="O11" s="36"/>
       <c r="P11" s="30"/>
       <c r="AC11" s="30"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="39"/>
+      <c r="A12" s="37"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -28211,12 +28194,12 @@
       <c r="K12" s="22"/>
       <c r="L12" s="22"/>
       <c r="M12" s="22"/>
-      <c r="O12" s="38"/>
+      <c r="O12" s="36"/>
       <c r="P12" s="22"/>
       <c r="AC12" s="22"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="40"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="30"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -28229,12 +28212,12 @@
       <c r="K13" s="30"/>
       <c r="L13" s="30"/>
       <c r="M13" s="30"/>
-      <c r="O13" s="38"/>
+      <c r="O13" s="36"/>
       <c r="P13" s="30"/>
       <c r="AC13" s="30"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="39"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="22"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
@@ -28247,12 +28230,12 @@
       <c r="K14" s="22"/>
       <c r="L14" s="22"/>
       <c r="M14" s="22"/>
-      <c r="O14" s="38"/>
+      <c r="O14" s="36"/>
       <c r="P14" s="22"/>
       <c r="AC14" s="22"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="40"/>
+      <c r="A15" s="38"/>
       <c r="B15" s="30"/>
       <c r="C15" s="30"/>
       <c r="D15" s="30"/>
@@ -28265,12 +28248,12 @@
       <c r="K15" s="30"/>
       <c r="L15" s="30"/>
       <c r="M15" s="30"/>
-      <c r="O15" s="38"/>
+      <c r="O15" s="36"/>
       <c r="P15" s="30"/>
       <c r="AC15" s="30"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="39"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
@@ -28283,12 +28266,12 @@
       <c r="K16" s="22"/>
       <c r="L16" s="22"/>
       <c r="M16" s="22"/>
-      <c r="O16" s="38"/>
+      <c r="O16" s="36"/>
       <c r="P16" s="22"/>
       <c r="AC16" s="22"/>
     </row>
     <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" s="40"/>
+      <c r="A17" s="38"/>
       <c r="B17" s="30"/>
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
@@ -28301,12 +28284,12 @@
       <c r="K17" s="30"/>
       <c r="L17" s="30"/>
       <c r="M17" s="30"/>
-      <c r="O17" s="38"/>
+      <c r="O17" s="36"/>
       <c r="P17" s="30"/>
       <c r="AC17" s="30"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="39"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="22"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
@@ -28319,12 +28302,12 @@
       <c r="K18" s="22"/>
       <c r="L18" s="22"/>
       <c r="M18" s="22"/>
-      <c r="O18" s="38"/>
+      <c r="O18" s="36"/>
       <c r="P18" s="22"/>
       <c r="AC18" s="22"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="40"/>
+      <c r="A19" s="38"/>
       <c r="B19" s="30"/>
       <c r="C19" s="30"/>
       <c r="D19" s="30"/>
@@ -28337,12 +28320,12 @@
       <c r="K19" s="30"/>
       <c r="L19" s="30"/>
       <c r="M19" s="30"/>
-      <c r="O19" s="38"/>
+      <c r="O19" s="36"/>
       <c r="P19" s="30"/>
       <c r="AC19" s="30"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="39"/>
+      <c r="A20" s="37"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
@@ -28355,12 +28338,12 @@
       <c r="K20" s="22"/>
       <c r="L20" s="22"/>
       <c r="M20" s="22"/>
-      <c r="O20" s="38"/>
+      <c r="O20" s="36"/>
       <c r="P20" s="22"/>
       <c r="AC20" s="22"/>
     </row>
     <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="40"/>
+      <c r="A21" s="38"/>
       <c r="B21" s="30"/>
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
@@ -28373,12 +28356,12 @@
       <c r="K21" s="30"/>
       <c r="L21" s="30"/>
       <c r="M21" s="30"/>
-      <c r="O21" s="38"/>
+      <c r="O21" s="36"/>
       <c r="P21" s="30"/>
       <c r="AC21" s="30"/>
     </row>
     <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" s="39"/>
+      <c r="A22" s="37"/>
       <c r="B22" s="22"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
@@ -28391,12 +28374,12 @@
       <c r="K22" s="22"/>
       <c r="L22" s="22"/>
       <c r="M22" s="22"/>
-      <c r="O22" s="38"/>
+      <c r="O22" s="36"/>
       <c r="P22" s="22"/>
       <c r="AC22" s="22"/>
     </row>
     <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="40"/>
+      <c r="A23" s="38"/>
       <c r="B23" s="30"/>
       <c r="C23" s="30"/>
       <c r="D23" s="30"/>
@@ -28409,12 +28392,12 @@
       <c r="K23" s="30"/>
       <c r="L23" s="30"/>
       <c r="M23" s="30"/>
-      <c r="O23" s="38"/>
+      <c r="O23" s="36"/>
       <c r="P23" s="30"/>
       <c r="AC23" s="30"/>
     </row>
     <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" s="39"/>
+      <c r="A24" s="37"/>
       <c r="B24" s="22"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
@@ -28427,12 +28410,12 @@
       <c r="K24" s="22"/>
       <c r="L24" s="22"/>
       <c r="M24" s="22"/>
-      <c r="O24" s="38"/>
+      <c r="O24" s="36"/>
       <c r="P24" s="22"/>
       <c r="AC24" s="22"/>
     </row>
     <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" s="40"/>
+      <c r="A25" s="38"/>
       <c r="B25" s="30"/>
       <c r="C25" s="30"/>
       <c r="D25" s="30"/>
@@ -28445,12 +28428,12 @@
       <c r="K25" s="30"/>
       <c r="L25" s="30"/>
       <c r="M25" s="30"/>
-      <c r="O25" s="38"/>
+      <c r="O25" s="36"/>
       <c r="P25" s="30"/>
       <c r="AC25" s="30"/>
     </row>
     <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" s="39"/>
+      <c r="A26" s="37"/>
       <c r="B26" s="22"/>
       <c r="C26" s="22"/>
       <c r="D26" s="22"/>
@@ -28463,12 +28446,12 @@
       <c r="K26" s="22"/>
       <c r="L26" s="22"/>
       <c r="M26" s="22"/>
-      <c r="O26" s="38"/>
+      <c r="O26" s="36"/>
       <c r="P26" s="22"/>
       <c r="AC26" s="22"/>
     </row>
     <row r="27" ht="12.75" customHeight="1">
-      <c r="A27" s="40"/>
+      <c r="A27" s="38"/>
       <c r="B27" s="30"/>
       <c r="C27" s="30"/>
       <c r="D27" s="30"/>
@@ -28481,12 +28464,12 @@
       <c r="K27" s="30"/>
       <c r="L27" s="30"/>
       <c r="M27" s="30"/>
-      <c r="O27" s="38"/>
+      <c r="O27" s="36"/>
       <c r="P27" s="30"/>
       <c r="AC27" s="30"/>
     </row>
     <row r="28" ht="12.75" customHeight="1">
-      <c r="A28" s="39"/>
+      <c r="A28" s="37"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
@@ -28499,12 +28482,12 @@
       <c r="K28" s="22"/>
       <c r="L28" s="22"/>
       <c r="M28" s="22"/>
-      <c r="O28" s="38"/>
+      <c r="O28" s="36"/>
       <c r="P28" s="22"/>
       <c r="AC28" s="22"/>
     </row>
     <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" s="40"/>
+      <c r="A29" s="38"/>
       <c r="B29" s="30"/>
       <c r="C29" s="30"/>
       <c r="D29" s="30"/>
@@ -28517,12 +28500,12 @@
       <c r="K29" s="30"/>
       <c r="L29" s="30"/>
       <c r="M29" s="30"/>
-      <c r="O29" s="38"/>
+      <c r="O29" s="36"/>
       <c r="P29" s="30"/>
       <c r="AC29" s="30"/>
     </row>
     <row r="30" ht="12.75" customHeight="1">
-      <c r="A30" s="39"/>
+      <c r="A30" s="37"/>
       <c r="B30" s="22"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
@@ -28535,12 +28518,12 @@
       <c r="K30" s="22"/>
       <c r="L30" s="22"/>
       <c r="M30" s="22"/>
-      <c r="O30" s="38"/>
+      <c r="O30" s="36"/>
       <c r="P30" s="22"/>
       <c r="AC30" s="22"/>
     </row>
     <row r="31" ht="12.75" customHeight="1">
-      <c r="A31" s="40"/>
+      <c r="A31" s="38"/>
       <c r="B31" s="30"/>
       <c r="C31" s="30"/>
       <c r="D31" s="30"/>
@@ -28553,12 +28536,12 @@
       <c r="K31" s="30"/>
       <c r="L31" s="30"/>
       <c r="M31" s="30"/>
-      <c r="O31" s="38"/>
+      <c r="O31" s="36"/>
       <c r="P31" s="30"/>
       <c r="AC31" s="30"/>
     </row>
     <row r="32" ht="12.75" customHeight="1">
-      <c r="A32" s="39"/>
+      <c r="A32" s="37"/>
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
       <c r="D32" s="22"/>
@@ -28571,12 +28554,12 @@
       <c r="K32" s="22"/>
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
-      <c r="O32" s="38"/>
+      <c r="O32" s="36"/>
       <c r="P32" s="22"/>
       <c r="AC32" s="22"/>
     </row>
     <row r="33" ht="12.75" customHeight="1">
-      <c r="A33" s="40"/>
+      <c r="A33" s="38"/>
       <c r="B33" s="30"/>
       <c r="C33" s="30"/>
       <c r="D33" s="30"/>
@@ -28589,12 +28572,12 @@
       <c r="K33" s="30"/>
       <c r="L33" s="30"/>
       <c r="M33" s="30"/>
-      <c r="O33" s="38"/>
+      <c r="O33" s="36"/>
       <c r="P33" s="30"/>
       <c r="AC33" s="30"/>
     </row>
     <row r="34" ht="12.75" customHeight="1">
-      <c r="A34" s="39"/>
+      <c r="A34" s="37"/>
       <c r="B34" s="22"/>
       <c r="C34" s="22"/>
       <c r="D34" s="22"/>
@@ -28607,12 +28590,12 @@
       <c r="K34" s="22"/>
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
-      <c r="O34" s="38"/>
+      <c r="O34" s="36"/>
       <c r="P34" s="22"/>
       <c r="AC34" s="22"/>
     </row>
     <row r="35" ht="12.75" customHeight="1">
-      <c r="A35" s="40"/>
+      <c r="A35" s="38"/>
       <c r="B35" s="30"/>
       <c r="C35" s="30"/>
       <c r="D35" s="30"/>
@@ -28625,12 +28608,12 @@
       <c r="K35" s="30"/>
       <c r="L35" s="30"/>
       <c r="M35" s="30"/>
-      <c r="O35" s="38"/>
+      <c r="O35" s="36"/>
       <c r="P35" s="30"/>
       <c r="AC35" s="30"/>
     </row>
     <row r="36" ht="12.75" customHeight="1">
-      <c r="A36" s="39"/>
+      <c r="A36" s="37"/>
       <c r="B36" s="22"/>
       <c r="C36" s="22"/>
       <c r="D36" s="22"/>
@@ -28643,12 +28626,12 @@
       <c r="K36" s="22"/>
       <c r="L36" s="22"/>
       <c r="M36" s="22"/>
-      <c r="O36" s="38"/>
+      <c r="O36" s="36"/>
       <c r="P36" s="22"/>
       <c r="AC36" s="22"/>
     </row>
     <row r="37" ht="12.75" customHeight="1">
-      <c r="A37" s="40"/>
+      <c r="A37" s="38"/>
       <c r="B37" s="30"/>
       <c r="C37" s="30"/>
       <c r="D37" s="30"/>
@@ -28661,12 +28644,12 @@
       <c r="K37" s="30"/>
       <c r="L37" s="30"/>
       <c r="M37" s="30"/>
-      <c r="O37" s="38"/>
+      <c r="O37" s="36"/>
       <c r="P37" s="30"/>
       <c r="AC37" s="30"/>
     </row>
     <row r="38" ht="12.75" customHeight="1">
-      <c r="A38" s="39"/>
+      <c r="A38" s="37"/>
       <c r="B38" s="22"/>
       <c r="C38" s="22"/>
       <c r="D38" s="22"/>
@@ -28679,12 +28662,12 @@
       <c r="K38" s="22"/>
       <c r="L38" s="22"/>
       <c r="M38" s="22"/>
-      <c r="O38" s="38"/>
+      <c r="O38" s="36"/>
       <c r="P38" s="22"/>
       <c r="AC38" s="22"/>
     </row>
     <row r="39" ht="12.75" customHeight="1">
-      <c r="A39" s="40"/>
+      <c r="A39" s="38"/>
       <c r="B39" s="30"/>
       <c r="C39" s="30"/>
       <c r="D39" s="30"/>
@@ -28697,12 +28680,12 @@
       <c r="K39" s="30"/>
       <c r="L39" s="30"/>
       <c r="M39" s="30"/>
-      <c r="O39" s="38"/>
+      <c r="O39" s="36"/>
       <c r="P39" s="30"/>
       <c r="AC39" s="30"/>
     </row>
     <row r="40" ht="12.75" customHeight="1">
-      <c r="A40" s="39"/>
+      <c r="A40" s="37"/>
       <c r="B40" s="22"/>
       <c r="C40" s="22"/>
       <c r="D40" s="22"/>
@@ -28715,12 +28698,12 @@
       <c r="K40" s="22"/>
       <c r="L40" s="22"/>
       <c r="M40" s="22"/>
-      <c r="O40" s="38"/>
+      <c r="O40" s="36"/>
       <c r="P40" s="22"/>
       <c r="AC40" s="22"/>
     </row>
     <row r="41" ht="12.75" customHeight="1">
-      <c r="A41" s="40"/>
+      <c r="A41" s="38"/>
       <c r="B41" s="30"/>
       <c r="C41" s="30"/>
       <c r="D41" s="30"/>
@@ -28733,12 +28716,12 @@
       <c r="K41" s="30"/>
       <c r="L41" s="30"/>
       <c r="M41" s="30"/>
-      <c r="O41" s="38"/>
+      <c r="O41" s="36"/>
       <c r="P41" s="30"/>
       <c r="AC41" s="30"/>
     </row>
     <row r="42" ht="12.75" customHeight="1">
-      <c r="A42" s="39"/>
+      <c r="A42" s="37"/>
       <c r="B42" s="22"/>
       <c r="C42" s="22"/>
       <c r="D42" s="22"/>
@@ -28751,12 +28734,12 @@
       <c r="K42" s="22"/>
       <c r="L42" s="22"/>
       <c r="M42" s="22"/>
-      <c r="O42" s="38"/>
+      <c r="O42" s="36"/>
       <c r="P42" s="22"/>
       <c r="AC42" s="22"/>
     </row>
     <row r="43" ht="12.75" customHeight="1">
-      <c r="A43" s="40"/>
+      <c r="A43" s="38"/>
       <c r="B43" s="30"/>
       <c r="C43" s="30"/>
       <c r="D43" s="30"/>
@@ -28769,12 +28752,12 @@
       <c r="K43" s="30"/>
       <c r="L43" s="30"/>
       <c r="M43" s="30"/>
-      <c r="O43" s="38"/>
+      <c r="O43" s="36"/>
       <c r="P43" s="30"/>
       <c r="AC43" s="30"/>
     </row>
     <row r="44" ht="12.75" customHeight="1">
-      <c r="A44" s="39"/>
+      <c r="A44" s="37"/>
       <c r="B44" s="22"/>
       <c r="C44" s="22"/>
       <c r="D44" s="22"/>
@@ -28787,12 +28770,12 @@
       <c r="K44" s="22"/>
       <c r="L44" s="22"/>
       <c r="M44" s="22"/>
-      <c r="O44" s="38"/>
+      <c r="O44" s="36"/>
       <c r="P44" s="22"/>
       <c r="AC44" s="22"/>
     </row>
     <row r="45" ht="12.75" customHeight="1">
-      <c r="A45" s="40"/>
+      <c r="A45" s="38"/>
       <c r="B45" s="30"/>
       <c r="C45" s="30"/>
       <c r="D45" s="30"/>
@@ -28805,12 +28788,12 @@
       <c r="K45" s="30"/>
       <c r="L45" s="30"/>
       <c r="M45" s="30"/>
-      <c r="O45" s="38"/>
+      <c r="O45" s="36"/>
       <c r="P45" s="30"/>
       <c r="AC45" s="30"/>
     </row>
     <row r="46" ht="12.75" customHeight="1">
-      <c r="A46" s="39"/>
+      <c r="A46" s="37"/>
       <c r="B46" s="22"/>
       <c r="C46" s="22"/>
       <c r="D46" s="22"/>
@@ -28823,12 +28806,12 @@
       <c r="K46" s="22"/>
       <c r="L46" s="22"/>
       <c r="M46" s="22"/>
-      <c r="O46" s="38"/>
+      <c r="O46" s="36"/>
       <c r="P46" s="22"/>
       <c r="AC46" s="22"/>
     </row>
     <row r="47" ht="12.75" customHeight="1">
-      <c r="A47" s="40"/>
+      <c r="A47" s="38"/>
       <c r="B47" s="30"/>
       <c r="C47" s="30"/>
       <c r="D47" s="30"/>
@@ -28841,12 +28824,12 @@
       <c r="K47" s="30"/>
       <c r="L47" s="30"/>
       <c r="M47" s="30"/>
-      <c r="O47" s="38"/>
+      <c r="O47" s="36"/>
       <c r="P47" s="30"/>
       <c r="AC47" s="30"/>
     </row>
     <row r="48" ht="12.75" customHeight="1">
-      <c r="A48" s="39"/>
+      <c r="A48" s="37"/>
       <c r="B48" s="22"/>
       <c r="C48" s="22"/>
       <c r="D48" s="22"/>
@@ -28859,12 +28842,12 @@
       <c r="K48" s="22"/>
       <c r="L48" s="22"/>
       <c r="M48" s="22"/>
-      <c r="O48" s="38"/>
+      <c r="O48" s="36"/>
       <c r="P48" s="22"/>
       <c r="AC48" s="22"/>
     </row>
     <row r="49" ht="12.75" customHeight="1">
-      <c r="A49" s="40"/>
+      <c r="A49" s="38"/>
       <c r="B49" s="30"/>
       <c r="C49" s="30"/>
       <c r="D49" s="30"/>
@@ -28877,12 +28860,12 @@
       <c r="K49" s="30"/>
       <c r="L49" s="30"/>
       <c r="M49" s="30"/>
-      <c r="O49" s="38"/>
+      <c r="O49" s="36"/>
       <c r="P49" s="30"/>
       <c r="AC49" s="30"/>
     </row>
     <row r="50" ht="12.75" customHeight="1">
-      <c r="A50" s="39"/>
+      <c r="A50" s="37"/>
       <c r="B50" s="22"/>
       <c r="C50" s="22"/>
       <c r="D50" s="22"/>
@@ -28895,12 +28878,12 @@
       <c r="K50" s="22"/>
       <c r="L50" s="22"/>
       <c r="M50" s="22"/>
-      <c r="O50" s="38"/>
+      <c r="O50" s="36"/>
       <c r="P50" s="22"/>
       <c r="AC50" s="22"/>
     </row>
     <row r="51" ht="12.75" customHeight="1">
-      <c r="A51" s="40"/>
+      <c r="A51" s="38"/>
       <c r="B51" s="30"/>
       <c r="C51" s="30"/>
       <c r="D51" s="30"/>
@@ -28913,12 +28896,12 @@
       <c r="K51" s="30"/>
       <c r="L51" s="30"/>
       <c r="M51" s="30"/>
-      <c r="O51" s="38"/>
+      <c r="O51" s="36"/>
       <c r="P51" s="30"/>
       <c r="AC51" s="30"/>
     </row>
     <row r="52" ht="12.75" customHeight="1">
-      <c r="A52" s="39"/>
+      <c r="A52" s="37"/>
       <c r="B52" s="22"/>
       <c r="C52" s="22"/>
       <c r="D52" s="22"/>
@@ -28931,12 +28914,12 @@
       <c r="K52" s="22"/>
       <c r="L52" s="22"/>
       <c r="M52" s="22"/>
-      <c r="O52" s="38"/>
+      <c r="O52" s="36"/>
       <c r="P52" s="22"/>
       <c r="AC52" s="22"/>
     </row>
     <row r="53" ht="12.75" customHeight="1">
-      <c r="A53" s="40"/>
+      <c r="A53" s="38"/>
       <c r="B53" s="30"/>
       <c r="C53" s="30"/>
       <c r="D53" s="30"/>
@@ -28949,12 +28932,12 @@
       <c r="K53" s="30"/>
       <c r="L53" s="30"/>
       <c r="M53" s="30"/>
-      <c r="O53" s="38"/>
+      <c r="O53" s="36"/>
       <c r="P53" s="30"/>
       <c r="AC53" s="30"/>
     </row>
     <row r="54" ht="12.75" customHeight="1">
-      <c r="A54" s="39"/>
+      <c r="A54" s="37"/>
       <c r="B54" s="22"/>
       <c r="C54" s="22"/>
       <c r="D54" s="22"/>
@@ -28967,12 +28950,12 @@
       <c r="K54" s="22"/>
       <c r="L54" s="22"/>
       <c r="M54" s="22"/>
-      <c r="O54" s="38"/>
+      <c r="O54" s="36"/>
       <c r="P54" s="22"/>
       <c r="AC54" s="22"/>
     </row>
     <row r="55" ht="12.75" customHeight="1">
-      <c r="A55" s="40"/>
+      <c r="A55" s="38"/>
       <c r="B55" s="30"/>
       <c r="C55" s="30"/>
       <c r="D55" s="30"/>
@@ -28985,12 +28968,12 @@
       <c r="K55" s="30"/>
       <c r="L55" s="30"/>
       <c r="M55" s="30"/>
-      <c r="O55" s="38"/>
+      <c r="O55" s="36"/>
       <c r="P55" s="30"/>
       <c r="AC55" s="30"/>
     </row>
     <row r="56" ht="12.75" customHeight="1">
-      <c r="A56" s="39"/>
+      <c r="A56" s="37"/>
       <c r="B56" s="22"/>
       <c r="C56" s="22"/>
       <c r="D56" s="22"/>
@@ -29003,12 +28986,12 @@
       <c r="K56" s="22"/>
       <c r="L56" s="22"/>
       <c r="M56" s="22"/>
-      <c r="O56" s="38"/>
+      <c r="O56" s="36"/>
       <c r="P56" s="22"/>
       <c r="AC56" s="22"/>
     </row>
     <row r="57" ht="12.75" customHeight="1">
-      <c r="A57" s="40"/>
+      <c r="A57" s="38"/>
       <c r="B57" s="30"/>
       <c r="C57" s="30"/>
       <c r="D57" s="30"/>
@@ -29021,12 +29004,12 @@
       <c r="K57" s="30"/>
       <c r="L57" s="30"/>
       <c r="M57" s="30"/>
-      <c r="O57" s="38"/>
+      <c r="O57" s="36"/>
       <c r="P57" s="30"/>
       <c r="AC57" s="30"/>
     </row>
     <row r="58" ht="12.75" customHeight="1">
-      <c r="A58" s="39"/>
+      <c r="A58" s="37"/>
       <c r="B58" s="22"/>
       <c r="C58" s="22"/>
       <c r="D58" s="22"/>
@@ -29039,12 +29022,12 @@
       <c r="K58" s="22"/>
       <c r="L58" s="22"/>
       <c r="M58" s="22"/>
-      <c r="O58" s="38"/>
+      <c r="O58" s="36"/>
       <c r="P58" s="22"/>
       <c r="AC58" s="22"/>
     </row>
     <row r="59" ht="12.75" customHeight="1">
-      <c r="A59" s="40"/>
+      <c r="A59" s="38"/>
       <c r="B59" s="30"/>
       <c r="C59" s="30"/>
       <c r="D59" s="30"/>
@@ -29057,12 +29040,12 @@
       <c r="K59" s="30"/>
       <c r="L59" s="30"/>
       <c r="M59" s="30"/>
-      <c r="O59" s="38"/>
+      <c r="O59" s="36"/>
       <c r="P59" s="30"/>
       <c r="AC59" s="30"/>
     </row>
     <row r="60" ht="12.75" customHeight="1">
-      <c r="A60" s="39"/>
+      <c r="A60" s="37"/>
       <c r="B60" s="22"/>
       <c r="C60" s="22"/>
       <c r="D60" s="22"/>
@@ -29075,12 +29058,12 @@
       <c r="K60" s="22"/>
       <c r="L60" s="22"/>
       <c r="M60" s="22"/>
-      <c r="O60" s="38"/>
+      <c r="O60" s="36"/>
       <c r="P60" s="22"/>
       <c r="AC60" s="22"/>
     </row>
     <row r="61" ht="12.75" customHeight="1">
-      <c r="A61" s="40"/>
+      <c r="A61" s="38"/>
       <c r="B61" s="30"/>
       <c r="C61" s="30"/>
       <c r="D61" s="30"/>
@@ -29093,12 +29076,12 @@
       <c r="K61" s="30"/>
       <c r="L61" s="30"/>
       <c r="M61" s="30"/>
-      <c r="O61" s="38"/>
+      <c r="O61" s="36"/>
       <c r="P61" s="30"/>
       <c r="AC61" s="30"/>
     </row>
     <row r="62" ht="12.75" customHeight="1">
-      <c r="A62" s="39"/>
+      <c r="A62" s="37"/>
       <c r="B62" s="22"/>
       <c r="C62" s="22"/>
       <c r="D62" s="22"/>
@@ -29111,12 +29094,12 @@
       <c r="K62" s="22"/>
       <c r="L62" s="22"/>
       <c r="M62" s="22"/>
-      <c r="O62" s="38"/>
+      <c r="O62" s="36"/>
       <c r="P62" s="22"/>
       <c r="AC62" s="22"/>
     </row>
     <row r="63" ht="12.75" customHeight="1">
-      <c r="A63" s="40"/>
+      <c r="A63" s="38"/>
       <c r="B63" s="30"/>
       <c r="C63" s="30"/>
       <c r="D63" s="30"/>
@@ -29129,12 +29112,12 @@
       <c r="K63" s="30"/>
       <c r="L63" s="30"/>
       <c r="M63" s="30"/>
-      <c r="O63" s="38"/>
+      <c r="O63" s="36"/>
       <c r="P63" s="30"/>
       <c r="AC63" s="30"/>
     </row>
     <row r="64" ht="12.75" customHeight="1">
-      <c r="A64" s="39"/>
+      <c r="A64" s="37"/>
       <c r="B64" s="22"/>
       <c r="C64" s="22"/>
       <c r="D64" s="22"/>
@@ -29147,12 +29130,12 @@
       <c r="K64" s="22"/>
       <c r="L64" s="22"/>
       <c r="M64" s="22"/>
-      <c r="O64" s="38"/>
+      <c r="O64" s="36"/>
       <c r="P64" s="22"/>
       <c r="AC64" s="22"/>
     </row>
     <row r="65" ht="12.75" customHeight="1">
-      <c r="A65" s="40"/>
+      <c r="A65" s="38"/>
       <c r="B65" s="30"/>
       <c r="C65" s="30"/>
       <c r="D65" s="30"/>
@@ -29165,12 +29148,12 @@
       <c r="K65" s="30"/>
       <c r="L65" s="30"/>
       <c r="M65" s="30"/>
-      <c r="O65" s="38"/>
+      <c r="O65" s="36"/>
       <c r="P65" s="30"/>
       <c r="AC65" s="30"/>
     </row>
     <row r="66" ht="12.75" customHeight="1">
-      <c r="A66" s="39"/>
+      <c r="A66" s="37"/>
       <c r="B66" s="22"/>
       <c r="C66" s="22"/>
       <c r="D66" s="22"/>
@@ -29183,12 +29166,12 @@
       <c r="K66" s="22"/>
       <c r="L66" s="22"/>
       <c r="M66" s="22"/>
-      <c r="O66" s="38"/>
+      <c r="O66" s="36"/>
       <c r="P66" s="22"/>
       <c r="AC66" s="22"/>
     </row>
     <row r="67" ht="12.75" customHeight="1">
-      <c r="A67" s="40"/>
+      <c r="A67" s="38"/>
       <c r="B67" s="30"/>
       <c r="C67" s="30"/>
       <c r="D67" s="30"/>
@@ -29201,12 +29184,12 @@
       <c r="K67" s="30"/>
       <c r="L67" s="30"/>
       <c r="M67" s="30"/>
-      <c r="O67" s="38"/>
+      <c r="O67" s="36"/>
       <c r="P67" s="30"/>
       <c r="AC67" s="30"/>
     </row>
     <row r="68" ht="12.75" customHeight="1">
-      <c r="A68" s="39"/>
+      <c r="A68" s="37"/>
       <c r="B68" s="22"/>
       <c r="C68" s="22"/>
       <c r="D68" s="22"/>
@@ -29219,12 +29202,12 @@
       <c r="K68" s="22"/>
       <c r="L68" s="22"/>
       <c r="M68" s="22"/>
-      <c r="O68" s="38"/>
+      <c r="O68" s="36"/>
       <c r="P68" s="22"/>
       <c r="AC68" s="22"/>
     </row>
     <row r="69" ht="12.75" customHeight="1">
-      <c r="A69" s="40"/>
+      <c r="A69" s="38"/>
       <c r="B69" s="30"/>
       <c r="C69" s="30"/>
       <c r="D69" s="30"/>
@@ -29237,12 +29220,12 @@
       <c r="K69" s="30"/>
       <c r="L69" s="30"/>
       <c r="M69" s="30"/>
-      <c r="O69" s="38"/>
+      <c r="O69" s="36"/>
       <c r="P69" s="30"/>
       <c r="AC69" s="30"/>
     </row>
     <row r="70" ht="12.75" customHeight="1">
-      <c r="A70" s="39"/>
+      <c r="A70" s="37"/>
       <c r="B70" s="22"/>
       <c r="C70" s="22"/>
       <c r="D70" s="22"/>
@@ -29255,12 +29238,12 @@
       <c r="K70" s="22"/>
       <c r="L70" s="22"/>
       <c r="M70" s="22"/>
-      <c r="O70" s="38"/>
+      <c r="O70" s="36"/>
       <c r="P70" s="22"/>
       <c r="AC70" s="22"/>
     </row>
     <row r="71" ht="12.75" customHeight="1">
-      <c r="A71" s="40"/>
+      <c r="A71" s="38"/>
       <c r="B71" s="30"/>
       <c r="C71" s="30"/>
       <c r="D71" s="30"/>
@@ -29273,12 +29256,12 @@
       <c r="K71" s="30"/>
       <c r="L71" s="30"/>
       <c r="M71" s="30"/>
-      <c r="O71" s="38"/>
+      <c r="O71" s="36"/>
       <c r="P71" s="30"/>
       <c r="AC71" s="30"/>
     </row>
     <row r="72" ht="12.75" customHeight="1">
-      <c r="A72" s="39"/>
+      <c r="A72" s="37"/>
       <c r="B72" s="22"/>
       <c r="C72" s="22"/>
       <c r="D72" s="22"/>
@@ -29291,12 +29274,12 @@
       <c r="K72" s="22"/>
       <c r="L72" s="22"/>
       <c r="M72" s="22"/>
-      <c r="O72" s="38"/>
+      <c r="O72" s="36"/>
       <c r="P72" s="22"/>
       <c r="AC72" s="22"/>
     </row>
     <row r="73" ht="12.75" customHeight="1">
-      <c r="A73" s="40"/>
+      <c r="A73" s="38"/>
       <c r="B73" s="30"/>
       <c r="C73" s="30"/>
       <c r="D73" s="30"/>
@@ -29309,12 +29292,12 @@
       <c r="K73" s="30"/>
       <c r="L73" s="30"/>
       <c r="M73" s="30"/>
-      <c r="O73" s="38"/>
+      <c r="O73" s="36"/>
       <c r="P73" s="30"/>
       <c r="AC73" s="30"/>
     </row>
     <row r="74" ht="12.75" customHeight="1">
-      <c r="A74" s="39"/>
+      <c r="A74" s="37"/>
       <c r="B74" s="22"/>
       <c r="C74" s="22"/>
       <c r="D74" s="22"/>
@@ -29327,12 +29310,12 @@
       <c r="K74" s="22"/>
       <c r="L74" s="22"/>
       <c r="M74" s="22"/>
-      <c r="O74" s="38"/>
+      <c r="O74" s="36"/>
       <c r="P74" s="22"/>
       <c r="AC74" s="22"/>
     </row>
     <row r="75" ht="12.75" customHeight="1">
-      <c r="A75" s="40"/>
+      <c r="A75" s="38"/>
       <c r="B75" s="30"/>
       <c r="C75" s="30"/>
       <c r="D75" s="30"/>
@@ -29345,7 +29328,7 @@
       <c r="K75" s="30"/>
       <c r="L75" s="30"/>
       <c r="M75" s="30"/>
-      <c r="O75" s="38"/>
+      <c r="O75" s="36"/>
       <c r="P75" s="30"/>
       <c r="AC75" s="30"/>
     </row>
@@ -30319,22 +30302,22 @@
         <v>117</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>203</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>204</v>
       </c>
       <c r="H1" s="10" t="s">
         <v>134</v>
@@ -30408,7 +30391,7 @@
       <c r="AE1" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="AF1" s="36" t="s">
+      <c r="AF1" s="34" t="s">
         <v>158</v>
       </c>
     </row>
@@ -30420,7 +30403,7 @@
         <v>106</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D2" s="27">
         <v>132416.32</v>
@@ -30429,12 +30412,12 @@
         <v>43987.643125</v>
       </c>
       <c r="F2" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="H2" s="36">
+      <c r="H2" s="34">
         <v>75.0</v>
       </c>
       <c r="I2" s="29">
@@ -32824,13 +32807,13 @@
         <v>117</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>209</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>210</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>134</v>
@@ -32904,27 +32887,27 @@
       <c r="AB1" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="AC1" s="36" t="s">
+      <c r="AC1" s="34" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="43">
+      <c r="C2" s="41">
         <v>2.101184477E7</v>
       </c>
-      <c r="D2" s="44">
+      <c r="D2" s="42">
         <v>44008.0</v>
       </c>
-      <c r="E2" s="36">
+      <c r="E2" s="34">
         <v>75.0</v>
       </c>
-      <c r="F2" s="43">
+      <c r="F2" s="41">
         <v>2.101184477E7</v>
       </c>
       <c r="G2" s="8">
@@ -32933,12 +32916,12 @@
       <c r="H2" s="8">
         <v>44012.0</v>
       </c>
-      <c r="I2" s="43">
+      <c r="I2" s="41">
         <v>2.101184477E7</v>
       </c>
       <c r="J2" s="13"/>
       <c r="K2" s="13"/>
-      <c r="L2" s="45">
+      <c r="L2" s="43">
         <v>1.0505922385E7</v>
       </c>
       <c r="M2" s="13"/>
@@ -32951,22 +32934,22 @@
       <c r="R2" s="13"/>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="45">
         <v>1.578213759E7</v>
       </c>
-      <c r="D3" s="48">
+      <c r="D3" s="46">
         <v>44008.0</v>
       </c>
-      <c r="E3" s="36">
+      <c r="E3" s="34">
         <v>75.0</v>
       </c>
-      <c r="F3" s="47">
+      <c r="F3" s="45">
         <v>1.578213759E7</v>
       </c>
       <c r="G3" s="8">
@@ -32975,12 +32958,12 @@
       <c r="H3" s="8">
         <v>44012.0</v>
       </c>
-      <c r="I3" s="47">
+      <c r="I3" s="45">
         <v>1.578213759E7</v>
       </c>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
-      <c r="L3" s="45">
+      <c r="L3" s="43">
         <v>1.578213759E7</v>
       </c>
       <c r="M3" s="13"/>
@@ -32991,22 +32974,22 @@
       <c r="R3" s="13"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="49">
+      <c r="C4" s="47">
         <v>1.0964770477E8</v>
       </c>
-      <c r="D4" s="44">
+      <c r="D4" s="42">
         <v>44008.0</v>
       </c>
-      <c r="E4" s="36">
+      <c r="E4" s="34">
         <v>75.0</v>
       </c>
-      <c r="F4" s="43">
+      <c r="F4" s="41">
         <v>9647704.77</v>
       </c>
       <c r="G4" s="8">
@@ -33015,12 +32998,12 @@
       <c r="H4" s="8">
         <v>44012.0</v>
       </c>
-      <c r="I4" s="43">
+      <c r="I4" s="41">
         <v>9647704.77</v>
       </c>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="45">
+      <c r="L4" s="43">
         <v>4823852.385</v>
       </c>
       <c r="M4" s="13"/>
@@ -33029,7 +33012,7 @@
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
       <c r="R4" s="13"/>
-      <c r="T4" s="45">
+      <c r="T4" s="43">
         <v>4823852.385</v>
       </c>
     </row>
@@ -33070,7 +33053,7 @@
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="K10" s="13"/>
-      <c r="M10" s="50"/>
+      <c r="M10" s="48"/>
       <c r="O10" s="13"/>
       <c r="Q10" s="13"/>
       <c r="R10" s="13"/>

</xml_diff>